<commit_message>
Actualización de los logt, task y sumtask.
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="totales" sheetId="1" state="visible" r:id="rId2"/>
@@ -516,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="3">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -536,55 +536,6 @@
       <right/>
       <top style="hair"/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -613,7 +564,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="32">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -661,70 +612,27 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -797,7 +705,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -810,7 +718,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>recursos!$F$1</c:f>
+              <c:f>'recursos-ciclo-1'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -833,9 +741,9 @@
           <c:marker/>
           <c:cat>
             <c:strRef>
-              <c:f>recursos!$A$2:$A$13</c:f>
+              <c:f>'recursos-ciclo-1'!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -847,75 +755,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>recursos!$F$2:$F$13</c:f>
+              <c:f>'recursos-ciclo-1'!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.186746987951807</c:v>
+                  <c:v>0.191616766467066</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.340361445783132</c:v>
+                  <c:v>0.344311377245509</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.409638554216867</c:v>
+                  <c:v>0.413173652694611</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.614457831325301</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.837349397590361</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0.616766467065868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -926,7 +786,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>recursos!$H$1</c:f>
+              <c:f>'recursos-ciclo-1'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -949,9 +809,9 @@
           <c:marker/>
           <c:cat>
             <c:strRef>
-              <c:f>recursos!$A$2:$A$13</c:f>
+              <c:f>'recursos-ciclo-1'!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -963,86 +823,38 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>recursos!$H$2:$H$13</c:f>
+              <c:f>'recursos-ciclo-1'!$H$2:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.108433734939759</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.108433734939759</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.108433734939759</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.108433734939759</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.108433734939759</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="6215064"/>
-        <c:axId val="81978594"/>
+        <c:axId val="7905354"/>
+        <c:axId val="66762409"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6215064"/>
+        <c:axId val="7905354"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81978594"/>
+        <c:crossAx val="66762409"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1064,7 +876,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81978594"/>
+        <c:axId val="66762409"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +893,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="6215064"/>
+        <c:crossAx val="7905354"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1113,7 +925,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1126,7 +938,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'recursos-ciclo-1'!$F$1</c:f>
+              <c:f>recursos!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1149,9 +961,9 @@
           <c:marker/>
           <c:cat>
             <c:strRef>
-              <c:f>'recursos-ciclo-1'!$A$2:$A$5</c:f>
+              <c:f>recursos!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1163,27 +975,75 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'recursos-ciclo-1'!$F$2:$F$5</c:f>
+              <c:f>recursos!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.186746987951807</c:v>
+                  <c:v>0.191616766467066</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.340361445783132</c:v>
+                  <c:v>0.344311377245509</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.409638554216867</c:v>
+                  <c:v>0.413173652694611</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.614457831325301</c:v>
+                  <c:v>0.616766467065868</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.838323353293413</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1194,7 +1054,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'recursos-ciclo-1'!$H$1</c:f>
+              <c:f>recursos!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1217,9 +1077,9 @@
           <c:marker/>
           <c:cat>
             <c:strRef>
-              <c:f>'recursos-ciclo-1'!$A$2:$A$5</c:f>
+              <c:f>recursos!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1231,38 +1091,86 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'recursos-ciclo-1'!$H$2:$H$5</c:f>
+              <c:f>recursos!$H$2:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.00903614457831325</c:v>
+                  <c:v>0.11377245508982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0331325301204819</c:v>
+                  <c:v>0.11377245508982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0963855421686747</c:v>
+                  <c:v>0.11377245508982</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.108433734939759</c:v>
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11377245508982</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11377245508982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="21470182"/>
-        <c:axId val="50872393"/>
+        <c:axId val="77806698"/>
+        <c:axId val="41858882"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="21470182"/>
+        <c:axId val="77806698"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50872393"/>
+        <c:crossAx val="41858882"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1284,7 +1192,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50872393"/>
+        <c:axId val="41858882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1301,7 +1209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="21470182"/>
+        <c:crossAx val="77806698"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1338,15 +1246,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:colOff>311760</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>207000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:colOff>213120</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1354,8 +1262,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="305280" y="2073240"/>
-        <a:ext cx="8751600" cy="3285360"/>
+        <a:off x="311760" y="3059640"/>
+        <a:ext cx="8796960" cy="3067560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1373,15 +1281,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>545760</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:colOff>288360</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>447480</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:colOff>189720</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1389,8 +1297,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="545760" y="1500840"/>
-        <a:ext cx="8751600" cy="3297600"/>
+        <a:off x="288360" y="1925280"/>
+        <a:ext cx="8796960" cy="3067920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1415,9 +1323,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.50588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.52941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="12.1725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1426,7 +1334,7 @@
       </c>
       <c r="B1" s="2" t="n">
         <f aca="false">SUM(_che)</f>
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1447,20 +1355,20 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I13" activeCellId="0" pane="topLeft" sqref="I13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.72549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.6980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="7.17254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="40.8627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.6823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="17.7098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.36078431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="17.7098039215686"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.74509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.9333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="7.2078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="41.0705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.7725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="17.8"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.4078431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="17.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="12.1725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1526,7 +1434,7 @@
       </c>
       <c r="G3" s="14" t="n">
         <f aca="false">F3/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H3" s="15" t="n">
         <v>1</v>
@@ -1555,7 +1463,7 @@
       </c>
       <c r="G4" s="14" t="n">
         <f aca="false">F4/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H4" s="13" t="n">
         <v>1</v>
@@ -1584,7 +1492,7 @@
       </c>
       <c r="G5" s="14" t="n">
         <f aca="false">F5/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H5" s="13" t="n">
         <v>1</v>
@@ -1611,7 +1519,7 @@
       </c>
       <c r="G6" s="14" t="n">
         <f aca="false">F6/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H6" s="13" t="n">
         <v>1</v>
@@ -1637,7 +1545,7 @@
       </c>
       <c r="G7" s="14" t="n">
         <f aca="false">F7/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H7" s="13" t="n">
         <v>1</v>
@@ -1662,11 +1570,11 @@
         <v>24</v>
       </c>
       <c r="F8" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="14" t="n">
         <f aca="false">F8/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H8" s="13" t="n">
         <v>1</v>
@@ -1697,7 +1605,7 @@
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">F9/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H9" s="13" t="n">
         <v>1</v>
@@ -1728,7 +1636,7 @@
       </c>
       <c r="G10" s="14" t="n">
         <f aca="false">F10/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H10" s="13" t="n">
         <v>1</v>
@@ -1754,7 +1662,7 @@
       </c>
       <c r="G11" s="14" t="n">
         <f aca="false">F11/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H11" s="13" t="n">
         <v>1</v>
@@ -1785,7 +1693,7 @@
       </c>
       <c r="G12" s="14" t="n">
         <f aca="false">F12/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H12" s="13" t="n">
         <v>1</v>
@@ -1816,7 +1724,7 @@
       </c>
       <c r="G13" s="14" t="n">
         <f aca="false">F13/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H13" s="13" t="n">
         <v>2</v>
@@ -1840,7 +1748,7 @@
       </c>
       <c r="G14" s="14" t="n">
         <f aca="false">F14/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H14" s="13" t="n">
         <v>2</v>
@@ -1866,7 +1774,7 @@
       </c>
       <c r="G15" s="14" t="n">
         <f aca="false">F15/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H15" s="13" t="n">
         <v>2</v>
@@ -1892,7 +1800,7 @@
       </c>
       <c r="G16" s="14" t="n">
         <f aca="false">F16/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H16" s="13" t="n">
         <v>2</v>
@@ -1918,7 +1826,7 @@
       </c>
       <c r="G17" s="14" t="n">
         <f aca="false">F17/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H17" s="13" t="n">
         <v>2</v>
@@ -1944,7 +1852,7 @@
       </c>
       <c r="G18" s="14" t="n">
         <f aca="false">F18/_vtdhe</f>
-        <v>0.036144578313253</v>
+        <v>0.0359281437125748</v>
       </c>
       <c r="H18" s="13" t="n">
         <v>3</v>
@@ -1970,7 +1878,7 @@
       </c>
       <c r="G19" s="14" t="n">
         <f aca="false">F19/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H19" s="13" t="n">
         <v>3</v>
@@ -1996,7 +1904,7 @@
       </c>
       <c r="G20" s="14" t="n">
         <f aca="false">F20/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H20" s="13" t="n">
         <v>3</v>
@@ -2022,7 +1930,7 @@
       </c>
       <c r="G21" s="14" t="n">
         <f aca="false">F21/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H21" s="16" t="n">
         <v>3</v>
@@ -2046,7 +1954,7 @@
       </c>
       <c r="G22" s="14" t="n">
         <f aca="false">F22/_vtdhe</f>
-        <v>0.0150602409638554</v>
+        <v>0.0149700598802395</v>
       </c>
       <c r="H22" s="13" t="n">
         <v>4</v>
@@ -2072,7 +1980,7 @@
       </c>
       <c r="G23" s="14" t="n">
         <f aca="false">F23/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H23" s="13" t="n">
         <v>4</v>
@@ -2098,7 +2006,7 @@
       </c>
       <c r="G24" s="14" t="n">
         <f aca="false">F24/_vtdhe</f>
-        <v>0.0301204819277108</v>
+        <v>0.029940119760479</v>
       </c>
       <c r="H24" s="13" t="n">
         <v>4</v>
@@ -2124,7 +2032,7 @@
       </c>
       <c r="G25" s="14" t="n">
         <f aca="false">F25/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H25" s="13" t="n">
         <v>4</v>
@@ -2150,7 +2058,7 @@
       </c>
       <c r="G26" s="14" t="n">
         <f aca="false">F26/_vtdhe</f>
-        <v>0.0301204819277108</v>
+        <v>0.029940119760479</v>
       </c>
       <c r="H26" s="13" t="n">
         <v>4</v>
@@ -2176,7 +2084,7 @@
       </c>
       <c r="G27" s="14" t="n">
         <f aca="false">F27/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H27" s="13" t="n">
         <v>4</v>
@@ -2202,7 +2110,7 @@
       </c>
       <c r="G28" s="14" t="n">
         <f aca="false">F28/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H28" s="13" t="n">
         <v>4</v>
@@ -2228,7 +2136,7 @@
       </c>
       <c r="G29" s="14" t="n">
         <f aca="false">F29/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H29" s="13" t="n">
         <v>4</v>
@@ -2254,7 +2162,7 @@
       </c>
       <c r="G30" s="14" t="n">
         <f aca="false">F30/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H30" s="13" t="n">
         <v>4</v>
@@ -2280,7 +2188,7 @@
       </c>
       <c r="G31" s="14" t="n">
         <f aca="false">F31/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H31" s="13" t="n">
         <v>5</v>
@@ -2306,7 +2214,7 @@
       </c>
       <c r="G32" s="14" t="n">
         <f aca="false">F32/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H32" s="13" t="n">
         <v>5</v>
@@ -2332,7 +2240,7 @@
       </c>
       <c r="G33" s="14" t="n">
         <f aca="false">F33/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H33" s="13" t="n">
         <v>5</v>
@@ -2358,7 +2266,7 @@
       </c>
       <c r="G34" s="14" t="n">
         <f aca="false">F34/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H34" s="13" t="n">
         <v>5</v>
@@ -2384,7 +2292,7 @@
       </c>
       <c r="G35" s="14" t="n">
         <f aca="false">F35/_vtdhe</f>
-        <v>0.036144578313253</v>
+        <v>0.0359281437125748</v>
       </c>
       <c r="H35" s="13" t="n">
         <v>5</v>
@@ -2410,7 +2318,7 @@
       </c>
       <c r="G36" s="14" t="n">
         <f aca="false">F36/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H36" s="13" t="n">
         <v>5</v>
@@ -2434,7 +2342,7 @@
       </c>
       <c r="G37" s="14" t="n">
         <f aca="false">F37/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H37" s="13" t="n">
         <v>5</v>
@@ -2460,7 +2368,7 @@
       </c>
       <c r="G38" s="14" t="n">
         <f aca="false">F38/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="H38" s="13" t="n">
         <v>5</v>
@@ -2486,7 +2394,7 @@
       </c>
       <c r="G39" s="14" t="n">
         <f aca="false">F39/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="H39" s="13" t="n">
         <v>5</v>
@@ -2510,7 +2418,7 @@
       </c>
       <c r="G40" s="14" t="n">
         <f aca="false">F40/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H40" s="13" t="n">
         <v>6</v>
@@ -2536,7 +2444,7 @@
       </c>
       <c r="G41" s="14" t="n">
         <f aca="false">F41/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="H41" s="13" t="n">
         <v>6</v>
@@ -2562,7 +2470,7 @@
       </c>
       <c r="G42" s="14" t="n">
         <f aca="false">F42/_vtdhe</f>
-        <v>0.0301204819277108</v>
+        <v>0.029940119760479</v>
       </c>
       <c r="H42" s="13" t="n">
         <v>6</v>
@@ -2584,7 +2492,7 @@
       </c>
       <c r="G43" s="14" t="n">
         <f aca="false">F43/_vtdhe</f>
-        <v>0.036144578313253</v>
+        <v>0.0359281437125748</v>
       </c>
       <c r="H43" s="13" t="n">
         <v>6</v>
@@ -2608,7 +2516,7 @@
       </c>
       <c r="G44" s="14" t="n">
         <f aca="false">F44/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="H44" s="13" t="n">
         <v>6</v>
@@ -2638,16 +2546,16 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="16.243137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.8117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.5921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="20.4313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.6823529411765"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="20.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="12.1725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
@@ -2689,11 +2597,11 @@
       </c>
       <c r="D2" s="19" t="n">
         <f aca="false">SUMIF(_cs, A2, _che)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="21" t="n">
         <f aca="false">SUMIF(_cs, A2, _cpidge)</f>
-        <v>0.186746987951807</v>
+        <v>0.191616766467066</v>
       </c>
       <c r="F2" s="21" t="inlineStr">
         <f aca="false">E2</f>
@@ -2703,7 +2611,7 @@
       </c>
       <c r="G2" s="21" t="n">
         <f aca="false">SUMIF(_cs, A2, _cpidgo)</f>
-        <v>0.108433734939759</v>
+        <v>0.11377245508982</v>
       </c>
       <c r="H2" s="21" t="inlineStr">
         <f aca="false">G2</f>
@@ -2732,7 +2640,7 @@
       </c>
       <c r="E3" s="21" t="n">
         <f aca="false">SUMIF(_cs, A3, _cpidge)</f>
-        <v>0.153614457831325</v>
+        <v>0.152694610778443</v>
       </c>
       <c r="F3" s="21" t="inlineStr">
         <f aca="false">E3+F2</f>
@@ -2771,7 +2679,7 @@
       </c>
       <c r="E4" s="21" t="n">
         <f aca="false">SUMIF(_cs, A4, _cpidge)</f>
-        <v>0.0692771084337349</v>
+        <v>0.0688622754491018</v>
       </c>
       <c r="F4" s="21" t="inlineStr">
         <f aca="false">E4+F3</f>
@@ -2810,7 +2718,7 @@
       </c>
       <c r="E5" s="21" t="n">
         <f aca="false">SUMIF(_cs, A5, _cpidge)</f>
-        <v>0.204819277108434</v>
+        <v>0.203592814371257</v>
       </c>
       <c r="F5" s="21" t="inlineStr">
         <f aca="false">E5+F4</f>
@@ -2849,7 +2757,7 @@
       </c>
       <c r="E6" s="21" t="n">
         <f aca="false">SUMIF(_cs, A6, _cpidge)</f>
-        <v>0.22289156626506</v>
+        <v>0.221556886227545</v>
       </c>
       <c r="F6" s="21" t="inlineStr">
         <f aca="false">E6+F5</f>
@@ -2888,7 +2796,7 @@
       </c>
       <c r="E7" s="21" t="n">
         <f aca="false">SUMIF(_cs, A7, _cpidge)</f>
-        <v>0.162650602409639</v>
+        <v>0.161676646706587</v>
       </c>
       <c r="F7" s="21" t="inlineStr">
         <f aca="false">E7+F6</f>
@@ -3160,26 +3068,26 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="S12" activeCellId="0" pane="topLeft" sqref="S12"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="J1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Q5" activeCellId="0" pane="topLeft" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.72549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.6980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="7.17254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="40.8627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="2" width="17.7098039215686"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="17.6823529411765"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="17.7098039215686"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="9.36078431372549"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="17" width="17.7098039215686"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.2980392156863"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="17" width="17.7098039215686"/>
-    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.74509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.9333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="7.2078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="41.0705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="2" width="17.8"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="17.7725490196078"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="17.8"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="9.4078431372549"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="17" width="17.8"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.3882352941176"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="17" width="17.8"/>
+    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.5921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -3312,44 +3220,36 @@
         <v>1</v>
       </c>
       <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28" t="n">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="n">
         <v>0.5</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29" t="n">
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27" t="n">
         <f aca="false">SUM(G4:K4)</f>
         <v>0.5</v>
       </c>
-      <c r="M4" s="30" t="n">
+      <c r="M4" s="28" t="n">
         <f aca="false">L4/_vtdhe</f>
-        <v>0.00301204819277108</v>
-      </c>
-      <c r="N4" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="31" t="n">
+        <v>0.0029940119760479</v>
+      </c>
+      <c r="N4" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="29" t="n">
         <v>41899</v>
       </c>
-      <c r="P4" s="32" t="n">
+      <c r="P4" s="29" t="n">
         <v>41899</v>
       </c>
-      <c r="Q4" s="33" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R4" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="34" t="n">
-        <v>41899</v>
-      </c>
-      <c r="T4" s="35" t="n">
-        <v>41899</v>
-      </c>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5" s="13">
-      <c r="A5" s="36" t="n">
+      <c r="A5" s="23" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -3360,49 +3260,39 @@
       <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39" t="n">
+      <c r="F5" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30" t="n">
         <v>0.5</v>
       </c>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="29" t="n">
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="27" t="n">
         <f aca="false">SUM(G5:K5)</f>
         <v>0.5</v>
       </c>
-      <c r="M5" s="30" t="n">
+      <c r="M5" s="28" t="n">
         <f aca="false">L5/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="N5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O5" s="40" t="n">
+      <c r="O5" s="31" t="n">
         <v>41899</v>
       </c>
-      <c r="P5" s="35" t="n">
+      <c r="P5" s="29" t="n">
         <v>41899</v>
       </c>
-      <c r="Q5" s="41" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="R5" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="34" t="n">
-        <v>41899</v>
-      </c>
-      <c r="T5" s="35" t="n">
-        <v>41899</v>
-      </c>
+      <c r="Q5" s="16"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6" s="13">
-      <c r="A6" s="36" t="n">
+      <c r="A6" s="23" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -3413,49 +3303,39 @@
       <c r="E6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39" t="n">
+      <c r="F6" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="27"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30" t="n">
         <v>0.5</v>
       </c>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="29" t="n">
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="27" t="n">
         <f aca="false">SUM(G6:K6)</f>
         <v>0.5</v>
       </c>
-      <c r="M6" s="30" t="n">
+      <c r="M6" s="28" t="n">
         <f aca="false">L6/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="N6" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="40" t="n">
+      <c r="O6" s="31" t="n">
         <v>41899</v>
       </c>
-      <c r="P6" s="35" t="n">
+      <c r="P6" s="29" t="n">
         <v>41899</v>
       </c>
-      <c r="Q6" s="41" t="n">
-        <f aca="false">25/60</f>
-        <v>0.416666666666667</v>
-      </c>
-      <c r="R6" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="40" t="n">
-        <v>41899</v>
-      </c>
-      <c r="T6" s="35" t="n">
-        <v>41899</v>
-      </c>
+      <c r="Q6" s="16"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7" s="13">
-      <c r="A7" s="36" t="n">
+      <c r="A7" s="23" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -3464,47 +3344,47 @@
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="37" t="n">
+      <c r="F7" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" s="29" t="n">
+      <c r="G7" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" s="27" t="n">
         <f aca="false">SUM(G7:K7)</f>
         <v>10</v>
       </c>
-      <c r="M7" s="30" t="n">
+      <c r="M7" s="28" t="n">
         <f aca="false">L7/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="N7" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="40" t="n">
+      <c r="O7" s="31" t="n">
         <v>41900</v>
       </c>
-      <c r="P7" s="35" t="n">
+      <c r="P7" s="29" t="n">
         <v>41900</v>
       </c>
-      <c r="Q7" s="41"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="35"/>
+      <c r="Q7" s="16"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="8" s="13">
-      <c r="A8" s="36" t="n">
+      <c r="A8" s="23" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -3517,51 +3397,41 @@
       <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="29" t="n">
+      <c r="F8" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="27" t="n">
         <f aca="false">SUM(G8:K8)</f>
         <v>2</v>
       </c>
-      <c r="M8" s="30" t="n">
+      <c r="M8" s="28" t="n">
         <f aca="false">L8/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="N8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O8" s="40" t="n">
+      <c r="O8" s="31" t="n">
         <v>41901</v>
       </c>
-      <c r="P8" s="35" t="n">
+      <c r="P8" s="29" t="n">
         <v>41901</v>
       </c>
-      <c r="Q8" s="41" t="n">
-        <f aca="false">(35+35)/60</f>
-        <v>1.16666666666667</v>
-      </c>
-      <c r="R8" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="S8" s="40" t="n">
-        <v>41905</v>
-      </c>
-      <c r="T8" s="35" t="n">
-        <v>41905</v>
-      </c>
+      <c r="Q8" s="16"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9" s="13">
-      <c r="A9" s="36" t="n">
+      <c r="A9" s="23" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -3572,49 +3442,41 @@
       <c r="E9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="29" t="n">
+      <c r="F9" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="H9" s="30" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="30" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="27" t="n">
         <f aca="false">SUM(G9:K9)</f>
-        <v>2</v>
-      </c>
-      <c r="M9" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" s="28" t="n">
         <f aca="false">L9/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="N9" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="40" t="n">
+      <c r="O9" s="31" t="n">
         <v>41902</v>
       </c>
-      <c r="P9" s="35" t="n">
+      <c r="P9" s="29" t="n">
         <v>41902</v>
       </c>
-      <c r="Q9" s="41" t="n">
-        <f aca="false">(45+72)/60</f>
-        <v>1.95</v>
-      </c>
-      <c r="R9" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="S9" s="40" t="n">
-        <v>41910</v>
-      </c>
-      <c r="T9" s="35" t="n">
-        <v>41912</v>
-      </c>
+      <c r="Q9" s="16"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="13">
-      <c r="A10" s="36" t="n">
+      <c r="A10" s="23" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -3627,56 +3489,47 @@
       <c r="E10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="37" t="n">
+      <c r="F10" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="G10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" s="29" t="n">
+      <c r="G10" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" s="27" t="n">
         <f aca="false">SUM(G10:K10)</f>
         <v>10</v>
       </c>
-      <c r="M10" s="30" t="n">
+      <c r="M10" s="28" t="n">
         <f aca="false">L10/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="N10" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O10" s="40" t="n">
+      <c r="O10" s="31" t="n">
         <v>41902</v>
       </c>
-      <c r="P10" s="35" t="n">
+      <c r="P10" s="29" t="n">
         <v>41902</v>
       </c>
-      <c r="Q10" s="41" t="n">
-        <v>13</v>
-      </c>
-      <c r="R10" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="S10" s="40" t="n">
-        <v>41917</v>
-      </c>
-      <c r="T10" s="35" t="n">
-        <v>41917</v>
-      </c>
+      <c r="Q10" s="16"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="11" s="13">
-      <c r="A11" s="36" t="n">
+      <c r="A11" s="23" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -3689,43 +3542,43 @@
       <c r="E11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="37" t="n">
+      <c r="F11" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="39"/>
-      <c r="L11" s="29" t="n">
+      <c r="G11" s="27"/>
+      <c r="H11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="30"/>
+      <c r="L11" s="27" t="n">
         <f aca="false">SUM(G11:K11)</f>
         <v>3</v>
       </c>
-      <c r="M11" s="30" t="n">
+      <c r="M11" s="28" t="n">
         <f aca="false">L11/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="N11" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O11" s="40" t="n">
+      <c r="O11" s="31" t="n">
         <v>41903</v>
       </c>
-      <c r="P11" s="35" t="n">
+      <c r="P11" s="29" t="n">
         <v>41903</v>
       </c>
-      <c r="Q11" s="41"/>
-      <c r="S11" s="40"/>
-      <c r="T11" s="35"/>
+      <c r="Q11" s="16"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="12" s="13">
-      <c r="A12" s="36" t="n">
+      <c r="A12" s="23" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -3738,49 +3591,39 @@
       <c r="E12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39" t="n">
+      <c r="F12" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30" t="n">
         <v>0.5</v>
       </c>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="29" t="n">
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="27" t="n">
         <f aca="false">SUM(G12:K12)</f>
         <v>0.5</v>
       </c>
-      <c r="M12" s="30" t="n">
+      <c r="M12" s="28" t="n">
         <f aca="false">L12/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="N12" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O12" s="40" t="n">
+      <c r="O12" s="31" t="n">
         <v>41903</v>
       </c>
-      <c r="P12" s="35" t="n">
+      <c r="P12" s="29" t="n">
         <v>41903</v>
       </c>
-      <c r="Q12" s="41" t="n">
-        <f aca="false">23/60</f>
-        <v>0.383333333333333</v>
-      </c>
-      <c r="R12" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="S12" s="40" t="n">
-        <v>41913</v>
-      </c>
-      <c r="T12" s="35" t="n">
-        <v>41913</v>
-      </c>
+      <c r="Q12" s="16"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="13" s="13">
-      <c r="A13" s="36" t="n">
+      <c r="A13" s="23" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -3793,45 +3636,36 @@
       <c r="E13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="M13" s="30" t="n">
+      <c r="F13" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" s="28" t="n">
         <f aca="false">L13/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="N13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O13" s="40" t="n">
+      <c r="O13" s="31" t="n">
         <v>41905</v>
       </c>
-      <c r="P13" s="35" t="n">
+      <c r="P13" s="29" t="n">
         <v>41905</v>
       </c>
-      <c r="Q13" s="41" t="n">
-        <v>1</v>
-      </c>
-      <c r="R13" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="S13" s="40" t="n">
-        <v>41921</v>
-      </c>
-      <c r="T13" s="35" t="n">
-        <v>41921</v>
-      </c>
+      <c r="Q13" s="16"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="13">
-      <c r="A14" s="36" t="n">
+      <c r="A14" s="23" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -3844,47 +3678,47 @@
       <c r="E14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="37" t="n">
+      <c r="F14" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="G14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K14" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="L14" s="29" t="n">
+      <c r="G14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="27" t="n">
         <f aca="false">SUM(G14:K14)</f>
         <v>10</v>
       </c>
-      <c r="M14" s="30" t="n">
+      <c r="M14" s="28" t="n">
         <f aca="false">L14/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="N14" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O14" s="40" t="n">
+      <c r="O14" s="31" t="n">
         <v>41906</v>
       </c>
-      <c r="P14" s="35" t="n">
+      <c r="P14" s="29" t="n">
         <v>41906</v>
       </c>
-      <c r="Q14" s="41"/>
-      <c r="S14" s="40"/>
-      <c r="T14" s="35"/>
+      <c r="Q14" s="16"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="15" s="13">
-      <c r="A15" s="36" t="n">
+      <c r="A15" s="23" t="n">
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -3895,47 +3729,47 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="37" t="n">
+      <c r="F15" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K15" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="L15" s="29" t="n">
+      <c r="G15" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="L15" s="27" t="n">
         <f aca="false">SUM(G15:K15)</f>
         <v>10</v>
       </c>
-      <c r="M15" s="30" t="n">
+      <c r="M15" s="28" t="n">
         <f aca="false">L15/_vtdhe</f>
-        <v>0.0602409638554217</v>
+        <v>0.0598802395209581</v>
       </c>
       <c r="N15" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O15" s="40" t="n">
+      <c r="O15" s="31" t="n">
         <v>41907</v>
       </c>
-      <c r="P15" s="35" t="n">
+      <c r="P15" s="29" t="n">
         <v>41907</v>
       </c>
-      <c r="Q15" s="41"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="35"/>
+      <c r="Q15" s="16"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="16" s="13">
-      <c r="A16" s="36" t="n">
+      <c r="A16" s="23" t="n">
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -3948,43 +3782,43 @@
       <c r="E16" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="37" t="n">
+      <c r="F16" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="39"/>
-      <c r="L16" s="29" t="n">
+      <c r="G16" s="27"/>
+      <c r="H16" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="27" t="n">
         <f aca="false">SUM(G16:K16)</f>
         <v>3</v>
       </c>
-      <c r="M16" s="30" t="n">
+      <c r="M16" s="28" t="n">
         <f aca="false">L16/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="N16" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O16" s="40" t="n">
+      <c r="O16" s="31" t="n">
         <v>41908</v>
       </c>
-      <c r="P16" s="35" t="n">
+      <c r="P16" s="29" t="n">
         <v>41908</v>
       </c>
-      <c r="Q16" s="41"/>
-      <c r="S16" s="40"/>
-      <c r="T16" s="35"/>
+      <c r="Q16" s="16"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="17" s="13">
-      <c r="A17" s="36" t="n">
+      <c r="A17" s="23" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -3997,39 +3831,39 @@
       <c r="E17" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39" t="n">
+      <c r="F17" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30" t="n">
         <v>0.5</v>
       </c>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="29" t="n">
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="27" t="n">
         <f aca="false">SUM(G17:K17)</f>
         <v>0.5</v>
       </c>
-      <c r="M17" s="30" t="n">
+      <c r="M17" s="28" t="n">
         <f aca="false">L17/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="N17" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O17" s="40" t="n">
+      <c r="O17" s="31" t="n">
         <v>41910</v>
       </c>
-      <c r="P17" s="35" t="n">
+      <c r="P17" s="29" t="n">
         <v>41910</v>
       </c>
-      <c r="Q17" s="41"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="35"/>
+      <c r="Q17" s="16"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="18" s="13">
-      <c r="A18" s="36" t="n">
+      <c r="A18" s="23" t="n">
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -4042,36 +3876,36 @@
       <c r="E18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="M18" s="30" t="n">
+      <c r="F18" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="M18" s="28" t="n">
         <f aca="false">L18/_vtdhe</f>
-        <v>0.0120481927710843</v>
+        <v>0.0119760479041916</v>
       </c>
       <c r="N18" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O18" s="40" t="n">
+      <c r="O18" s="31" t="n">
         <v>41912</v>
       </c>
-      <c r="P18" s="35" t="n">
+      <c r="P18" s="29" t="n">
         <v>41912</v>
       </c>
-      <c r="Q18" s="41"/>
-      <c r="S18" s="40"/>
-      <c r="T18" s="35"/>
+      <c r="Q18" s="16"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="13">
-      <c r="A19" s="36" t="n">
+      <c r="A19" s="23" t="n">
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -4084,43 +3918,43 @@
       <c r="E19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="37" t="n">
+      <c r="F19" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" s="29" t="n">
+      <c r="G19" s="27"/>
+      <c r="H19" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="27" t="n">
         <f aca="false">SUM(G19:K19)</f>
         <v>3</v>
       </c>
-      <c r="M19" s="30" t="n">
+      <c r="M19" s="28" t="n">
         <f aca="false">L19/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="N19" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="O19" s="40" t="n">
+      <c r="O19" s="31" t="n">
         <v>41913</v>
       </c>
-      <c r="P19" s="35" t="n">
+      <c r="P19" s="29" t="n">
         <v>41913</v>
       </c>
-      <c r="Q19" s="41"/>
-      <c r="S19" s="40"/>
-      <c r="T19" s="35"/>
+      <c r="Q19" s="16"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="20" s="13">
-      <c r="A20" s="36" t="n">
+      <c r="A20" s="23" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -4133,43 +3967,43 @@
       <c r="E20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="37" t="n">
+      <c r="F20" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="39"/>
-      <c r="L20" s="29" t="n">
+      <c r="G20" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="27" t="n">
         <f aca="false">SUM(G20:K20)</f>
         <v>3</v>
       </c>
-      <c r="M20" s="30" t="n">
+      <c r="M20" s="28" t="n">
         <f aca="false">L20/_vtdhe</f>
-        <v>0.0180722891566265</v>
+        <v>0.0179640718562874</v>
       </c>
       <c r="N20" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="O20" s="40" t="n">
+      <c r="O20" s="31" t="n">
         <v>41913</v>
       </c>
-      <c r="P20" s="35" t="n">
+      <c r="P20" s="29" t="n">
         <v>41913</v>
       </c>
-      <c r="Q20" s="41"/>
-      <c r="S20" s="40"/>
-      <c r="T20" s="35"/>
+      <c r="Q20" s="16"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="21" s="13">
-      <c r="A21" s="36" t="n">
+      <c r="A21" s="23" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -4182,79 +4016,79 @@
       <c r="E21" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39" t="n">
+      <c r="F21" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="27"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30" t="n">
         <v>0.5</v>
       </c>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="29" t="n">
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="27" t="n">
         <f aca="false">SUM(G21:K21)</f>
         <v>0.5</v>
       </c>
-      <c r="M21" s="30" t="n">
+      <c r="M21" s="28" t="n">
         <f aca="false">L21/_vtdhe</f>
-        <v>0.00301204819277108</v>
+        <v>0.0029940119760479</v>
       </c>
       <c r="N21" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="O21" s="40" t="n">
+      <c r="O21" s="31" t="n">
         <v>41913</v>
       </c>
-      <c r="P21" s="35" t="n">
+      <c r="P21" s="29" t="n">
         <v>41913</v>
       </c>
-      <c r="Q21" s="41"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="35"/>
+      <c r="Q21" s="16"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="29"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="22" s="13">
-      <c r="A22" s="42" t="n">
+      <c r="A22" s="23" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43" t="s">
+      <c r="D22" s="24"/>
+      <c r="E22" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="46"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="M22" s="48" t="n">
+      <c r="F22" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="M22" s="28" t="n">
         <f aca="false">L22/_vtdhe</f>
-        <v>0.0120481927710843</v>
-      </c>
-      <c r="N22" s="49" t="n">
+        <v>0.0119760479041916</v>
+      </c>
+      <c r="N22" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="O22" s="50" t="n">
+      <c r="O22" s="29" t="n">
         <v>41915</v>
       </c>
-      <c r="P22" s="51" t="n">
+      <c r="P22" s="29" t="n">
         <v>41915</v>
       </c>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="50"/>
-      <c r="T22" s="51"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4280,17 +4114,17 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H12" activeCellId="0" pane="topLeft" sqref="H12"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H10" activeCellId="0" pane="topLeft" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="16.243137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.8117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.5921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="20.4313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.6823529411765"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="20.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="12.1725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
@@ -4332,11 +4166,11 @@
       </c>
       <c r="D2" s="19" t="n">
         <f aca="false">SUMIF(_cs, A2, _che)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="21" t="n">
         <f aca="false">SUMIF(_cs, A2, _cpidge)</f>
-        <v>0.186746987951807</v>
+        <v>0.191616766467066</v>
       </c>
       <c r="F2" s="21" t="inlineStr">
         <f aca="false">E2</f>
@@ -4346,7 +4180,7 @@
       </c>
       <c r="G2" s="21" t="n">
         <f aca="false">SUMIF(_cc1s, A2, _cc1pidge)</f>
-        <v>0.00903614457831325</v>
+        <v>0</v>
       </c>
       <c r="H2" s="21" t="inlineStr">
         <f aca="false">G2</f>
@@ -4375,7 +4209,7 @@
       </c>
       <c r="E3" s="21" t="n">
         <f aca="false">SUMIF(_cs, A3, _cpidge)</f>
-        <v>0.153614457831325</v>
+        <v>0.152694610778443</v>
       </c>
       <c r="F3" s="21" t="inlineStr">
         <f aca="false">E3+F2</f>
@@ -4385,7 +4219,7 @@
       </c>
       <c r="G3" s="21" t="n">
         <f aca="false">SUMIF(_cc1s, A3, _cc1pidge)</f>
-        <v>0.0240963855421687</v>
+        <v>0</v>
       </c>
       <c r="H3" s="21" t="inlineStr">
         <f aca="false">G3+H2</f>
@@ -4414,7 +4248,7 @@
       </c>
       <c r="E4" s="21" t="n">
         <f aca="false">SUMIF(_cs, A4, _cpidge)</f>
-        <v>0.0692771084337349</v>
+        <v>0.0688622754491018</v>
       </c>
       <c r="F4" s="21" t="inlineStr">
         <f aca="false">E4+F3</f>
@@ -4424,7 +4258,7 @@
       </c>
       <c r="G4" s="21" t="n">
         <f aca="false">SUMIF(_cc1s, A4, _cc1pidge)</f>
-        <v>0.0632530120481928</v>
+        <v>0</v>
       </c>
       <c r="H4" s="21" t="inlineStr">
         <f aca="false">G4+H3</f>
@@ -4453,7 +4287,7 @@
       </c>
       <c r="E5" s="21" t="n">
         <f aca="false">SUMIF(_cs, A5, _cpidge)</f>
-        <v>0.204819277108434</v>
+        <v>0.203592814371257</v>
       </c>
       <c r="F5" s="21" t="inlineStr">
         <f aca="false">E5+F4</f>
@@ -4463,7 +4297,7 @@
       </c>
       <c r="G5" s="21" t="n">
         <f aca="false">SUMIF(_cc1s, A5, _cc1pidge)</f>
-        <v>0.0120481927710843</v>
+        <v>0</v>
       </c>
       <c r="H5" s="21" t="inlineStr">
         <f aca="false">G5+H4</f>

</xml_diff>

<commit_message>
Versión final del documento de requerimientos.
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="439" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="439" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="tareas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
   <si>
     <t>Id</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Semana</t>
   </si>
   <si>
-    <t>Experimiento GitHub #1.</t>
+    <t>Ver video tutorial de GitHub.</t>
   </si>
   <si>
     <t>Realizar el lanzamiento del ciclo #1 de TSPi.</t>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Porcentaje individual de ganacias obtenidas</t>
+  </si>
+  <si>
+    <t>Horas Trabajadas</t>
+  </si>
+  <si>
+    <t>Totales</t>
   </si>
 </sst>
 </file>
@@ -231,7 +237,7 @@
     <numFmt formatCode="@" numFmtId="166"/>
     <numFmt formatCode="MM/DD/YYYY" numFmtId="167"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -272,6 +278,11 @@
       <family val="1"/>
       <color rgb="00000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="13"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -340,7 +351,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -426,6 +437,11 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -498,10 +514,28 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300"/>
+              <a:t>Ganacias Estimadas vs Ganacias Obtenidas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -511,7 +545,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'recursos-ciclo1'!$F$1</c:f>
+              <c:f>'recursos-ciclo1'!$F$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -556,13 +590,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.217522658610272</c:v>
+                  <c:v>0.351219512195122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.419939577039275</c:v>
+                  <c:v>0.678048780487805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.619335347432024</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,7 +607,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'recursos-ciclo1'!$H$1</c:f>
+              <c:f>'recursos-ciclo1'!$I$1:$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -613,29 +647,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'recursos-ciclo1'!$H$2:$H$4</c:f>
+              <c:f>'recursos-ciclo1'!$I$2:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0936555891238671</c:v>
+                  <c:v>0.151219512195122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.175226586102719</c:v>
+                  <c:v>0.282926829268293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.392749244712991</c:v>
+                  <c:v>0.634146341463415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82622093"/>
-        <c:axId val="85619649"/>
+        <c:axId val="35292534"/>
+        <c:axId val="74360889"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82622093"/>
+        <c:axId val="35292534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85619649"/>
+        <c:crossAx val="74360889"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -657,7 +691,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85619649"/>
+        <c:axId val="74360889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,8 +708,440 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82622093"/>
+        <c:crossAx val="35292534"/>
         <c:crossesAt val="0"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:spPr/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300"/>
+              <a:t>Horas Estimadas vs Horas Trabajadas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'recursos-ciclo1'!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Trabajadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'recursos-ciclo1'!$G$2:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>19.5166666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.1166666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.8833333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="96533322"/>
+        <c:axId val="19260892"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="96533322"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="19260892"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="19260892"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96533322"/>
+        <c:crosses val="autoZero"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:spPr/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300"/>
+              <a:t>Ganancias Estimadas vs Ganancias Obtenidas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje Individual de Ganacias Estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'recursos-ciclo1'!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.351219512195122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.326829268292683</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.321951219512195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje Individual de Ganancias Obtenidas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'recursos-ciclo1'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'recursos-ciclo1'!$H$2:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.151219512195122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.131707317073171</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.351219512195122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="92886555"/>
+        <c:axId val="96787227"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="92886555"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96787227"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96787227"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92886555"/>
+        <c:crosses val="autoZero"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -711,15 +1177,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>781920</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:colOff>31680</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1036800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>90000</xdr:rowOff>
+      <xdr:colOff>282960</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -727,12 +1193,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="781920" y="1807560"/>
-        <a:ext cx="7894440" cy="2621160"/>
+        <a:off x="31680" y="1517040"/>
+        <a:ext cx="7930080" cy="2794320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>391680</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1445400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>65880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="391680" y="4835160"/>
+        <a:ext cx="5762160" cy="3241800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647280</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>87480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>458280</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6840720" y="4780440"/>
+        <a:ext cx="5752080" cy="3241800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -748,19 +1274,19 @@
   </sheetPr>
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F1" activeCellId="0" pane="topLeft" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="39.8666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="39.8666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="40.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="40.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.3607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1657,16 +2183,16 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C26" activeCellId="0" pane="topLeft" sqref="C26"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="12.4823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="16.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="19.3725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="23" width="21.0470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="21" width="12.4823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="12.5450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="16.8235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="19.4705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="23" width="21.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="21" width="12.5450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
@@ -1707,22 +2233,12 @@
         <v>35</v>
       </c>
       <c r="D2" s="25" t="n">
-        <f aca="false">SUMIF(tareas!H3:H45,A2,tareas!F3:F45)</f>
+        <f aca="false">'recursos-ciclo1'!D2</f>
         <v>36</v>
       </c>
-      <c r="E2" s="27" t="inlineStr">
-        <f aca="false">'recursos-ciclo1'!E2</f>
-        <is>
-          <t/>
-        </is>
-      </c>
+      <c r="E2" s="27"/>
       <c r="F2" s="27"/>
-      <c r="G2" s="27" t="inlineStr">
-        <f aca="false">'recursos-ciclo1'!G2</f>
-        <is>
-          <t/>
-        </is>
-      </c>
+      <c r="G2" s="27"/>
       <c r="H2" s="27"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
@@ -1740,22 +2256,12 @@
         <v>35</v>
       </c>
       <c r="D3" s="25" t="n">
-        <f aca="false">SUMIF(tareas!H3:H45,A3,tareas!F3:F45)</f>
+        <f aca="false">'recursos-ciclo1'!D3</f>
         <v>33.5</v>
       </c>
-      <c r="E3" s="27" t="inlineStr">
-        <f aca="false">'recursos-ciclo1'!E3</f>
-        <is>
-          <t/>
-        </is>
-      </c>
+      <c r="E3" s="27"/>
       <c r="F3" s="27"/>
-      <c r="G3" s="27" t="inlineStr">
-        <f aca="false">'recursos-ciclo1'!G3</f>
-        <is>
-          <t/>
-        </is>
-      </c>
+      <c r="G3" s="27"/>
       <c r="H3" s="27"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
@@ -1773,22 +2279,12 @@
         <v>35</v>
       </c>
       <c r="D4" s="25" t="n">
-        <f aca="false">SUMIF(tareas!H3:H45,A4,tareas!F3:F45)</f>
+        <f aca="false">'recursos-ciclo1'!D4</f>
         <v>33</v>
       </c>
-      <c r="E4" s="27" t="inlineStr">
-        <f aca="false">'recursos-ciclo1'!E4</f>
-        <is>
-          <t/>
-        </is>
-      </c>
+      <c r="E4" s="27"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="27" t="inlineStr">
-        <f aca="false">'recursos-ciclo1'!G4</f>
-        <is>
-          <t/>
-        </is>
-      </c>
+      <c r="G4" s="27"/>
       <c r="H4" s="27"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
@@ -1805,10 +2301,7 @@
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D5" s="25" t="n">
-        <f aca="false">SUMIF(tareas!H3:H45,A5,tareas!F3:F45)</f>
-        <v>37.5</v>
-      </c>
+      <c r="D5" s="25"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
@@ -1828,10 +2321,7 @@
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D6" s="25" t="n">
-        <f aca="false">SUMIF(tareas!H3:H45,A6,tareas!F3:F45)</f>
-        <v>25.5</v>
-      </c>
+      <c r="D6" s="25"/>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -1975,26 +2465,26 @@
   </sheetPr>
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="O1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="R1" activeCellId="0" pane="topLeft" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="39.8666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="39.8666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="2.66666666666667"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="19.9333333333333"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="2.66666666666667"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="4" width="2.66666666666667"/>
-    <col collapsed="false" hidden="false" max="24" min="20" style="4" width="19.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="4" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="40.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="40.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="21.3607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="2.68627450980392"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="20.0313725490196"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="2.68627450980392"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="21.3607843137255"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="4" width="2.68627450980392"/>
+    <col collapsed="false" hidden="false" max="24" min="20" style="4" width="20.0313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="4" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -2033,8 +2523,8 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="28" t="n">
-        <f aca="false">tareas!F1</f>
-        <v>165.5</v>
+        <f aca="false">SUM(F4:F27)</f>
+        <v>102.5</v>
       </c>
       <c r="G2" s="9" t="inlineStr">
         <f aca="false">SUM(G4:G27)</f>
@@ -2175,7 +2665,7 @@
       </c>
       <c r="G4" s="9" t="n">
         <f aca="false">F4/F2</f>
-        <v>0.0453172205438066</v>
+        <v>0.0731707317073171</v>
       </c>
       <c r="H4" s="14" t="n">
         <v>1</v>
@@ -2197,10 +2687,12 @@
       </c>
       <c r="P4" s="1" t="n">
         <f aca="false">SUM(T4:X4)</f>
-        <v>4.46666666666666</v>
+        <v>4.46666666666667</v>
       </c>
       <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
+      <c r="R4" s="29" t="n">
+        <v>1</v>
+      </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="n">
@@ -2235,7 +2727,7 @@
       </c>
       <c r="G5" s="9" t="n">
         <f aca="false">F5/F2</f>
-        <v>0.0302114803625378</v>
+        <v>0.0487804878048781</v>
       </c>
       <c r="H5" s="14" t="n">
         <v>1</v>
@@ -2257,7 +2749,7 @@
       </c>
       <c r="P5" s="1" t="n">
         <f aca="false">SUM(T5:X5)</f>
-        <v>5.08333333333335</v>
+        <v>5.08333333333333</v>
       </c>
       <c r="Q5" s="3" t="inlineStr">
         <f aca="false">G5</f>
@@ -2305,7 +2797,7 @@
       </c>
       <c r="G6" s="9" t="n">
         <f aca="false">F6/F2</f>
-        <v>0.0302114803625378</v>
+        <v>0.0487804878048781</v>
       </c>
       <c r="H6" s="14" t="n">
         <v>1</v>
@@ -2375,7 +2867,7 @@
       </c>
       <c r="G7" s="9" t="n">
         <f aca="false">F7/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H7" s="14" t="n">
         <v>1</v>
@@ -2421,7 +2913,7 @@
       </c>
       <c r="G8" s="9" t="n">
         <f aca="false">F8/F2</f>
-        <v>0.00302114803625378</v>
+        <v>0.00487804878048781</v>
       </c>
       <c r="H8" s="19" t="n">
         <v>1</v>
@@ -2471,7 +2963,7 @@
       </c>
       <c r="G9" s="9" t="n">
         <f aca="false">F9/F2</f>
-        <v>0.00302114803625378</v>
+        <v>0.00487804878048781</v>
       </c>
       <c r="H9" s="18" t="n">
         <v>1</v>
@@ -2521,7 +3013,7 @@
       </c>
       <c r="G10" s="9" t="n">
         <f aca="false">F10/F2</f>
-        <v>0.00302114803625378</v>
+        <v>0.00487804878048781</v>
       </c>
       <c r="H10" s="18" t="n">
         <v>1</v>
@@ -2571,7 +3063,7 @@
       </c>
       <c r="G11" s="9" t="n">
         <f aca="false">F11/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H11" s="18" t="n">
         <v>1</v>
@@ -2622,7 +3114,7 @@
       </c>
       <c r="G12" s="9" t="n">
         <f aca="false">F12/F2</f>
-        <v>0.0181268882175227</v>
+        <v>0.0292682926829268</v>
       </c>
       <c r="H12" s="18" t="n">
         <v>1</v>
@@ -2677,7 +3169,7 @@
       </c>
       <c r="G13" s="9" t="n">
         <f aca="false">F13/F2</f>
-        <v>0.0604229607250755</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="H13" s="18" t="n">
         <v>1</v>
@@ -2702,7 +3194,9 @@
         <v>1.86666666666667</v>
       </c>
       <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
+      <c r="R13" s="30" t="n">
+        <v>1</v>
+      </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
       <c r="U13" s="18"/>
@@ -2725,7 +3219,7 @@
       </c>
       <c r="G14" s="3" t="n">
         <f aca="false">F14/F2</f>
-        <v>0.0906344410876133</v>
+        <v>0.146341463414634</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>2</v>
@@ -2750,7 +3244,9 @@
         <v>2.83333333333333</v>
       </c>
       <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
+      <c r="R14" s="29" t="n">
+        <v>2</v>
+      </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1" t="n">
         <f aca="false">80/60</f>
@@ -2779,7 +3275,7 @@
       </c>
       <c r="G15" s="9" t="n">
         <f aca="false">F15/F2</f>
-        <v>0.0604229607250755</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="H15" s="18" t="n">
         <v>2</v>
@@ -2849,7 +3345,7 @@
       </c>
       <c r="G16" s="9" t="n">
         <f aca="false">F16/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H16" s="18" t="n">
         <v>2</v>
@@ -2913,7 +3409,7 @@
       </c>
       <c r="G17" s="9" t="n">
         <f aca="false">F17/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H17" s="18" t="n">
         <v>2</v>
@@ -2950,7 +3446,7 @@
       </c>
       <c r="G18" s="9" t="n">
         <f aca="false">F18/F2</f>
-        <v>0.0241691842900302</v>
+        <v>0.0390243902439024</v>
       </c>
       <c r="H18" s="18" t="n">
         <v>2</v>
@@ -2989,7 +3485,7 @@
       </c>
       <c r="G19" s="9" t="n">
         <f aca="false">F19/F2</f>
-        <v>0.00302114803625378</v>
+        <v>0.00487804878048781</v>
       </c>
       <c r="H19" s="18" t="n">
         <v>2</v>
@@ -3038,7 +3534,7 @@
       </c>
       <c r="G20" s="9" t="n">
         <f aca="false">F20/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H20" s="18" t="n">
         <v>3</v>
@@ -3089,7 +3585,7 @@
       </c>
       <c r="G21" s="9" t="n">
         <f aca="false">F21/F2</f>
-        <v>0.0604229607250755</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="H21" s="18" t="n">
         <v>3</v>
@@ -3111,7 +3607,7 @@
       </c>
       <c r="P21" s="1" t="n">
         <f aca="false">SUM(T21:X21)</f>
-        <v>8.16666666666665</v>
+        <v>8.16666666666667</v>
       </c>
       <c r="Q21" s="31" t="inlineStr">
         <f aca="false">G21</f>
@@ -3156,7 +3652,7 @@
       </c>
       <c r="G22" s="9" t="n">
         <f aca="false">F22/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>3</v>
@@ -3211,7 +3707,7 @@
       </c>
       <c r="G23" s="9" t="n">
         <f aca="false">F23/F2</f>
-        <v>0.0181268882175227</v>
+        <v>0.0292682926829268</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>3</v>
@@ -3269,7 +3765,7 @@
       </c>
       <c r="G24" s="9" t="n">
         <f aca="false">F24/F2</f>
-        <v>0.0120845921450151</v>
+        <v>0.0195121951219512</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>3</v>
@@ -3318,7 +3814,7 @@
       </c>
       <c r="G25" s="9" t="n">
         <f aca="false">F25/F2</f>
-        <v>0.0241691842900302</v>
+        <v>0.0390243902439024</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>3</v>
@@ -3364,7 +3860,7 @@
       </c>
       <c r="G26" s="9" t="n">
         <f aca="false">F26/F2</f>
-        <v>0.0302114803625378</v>
+        <v>0.0487804878048781</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>3</v>
@@ -3431,7 +3927,7 @@
       </c>
       <c r="G27" s="9" t="n">
         <f aca="false">F27/F2</f>
-        <v>0.0302114803625378</v>
+        <v>0.0487804878048781</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>3</v>
@@ -3456,7 +3952,9 @@
         <v>0</v>
       </c>
       <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
+      <c r="R27" s="29" t="n">
+        <v>3</v>
+      </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -3492,19 +3990,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F16" activeCellId="0" pane="topLeft" sqref="F16"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K28" activeCellId="0" pane="topLeft" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="12.4823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="16.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="19.3725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="23" width="21.0470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="21" width="12.4823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="12.5450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="16.8235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="19.4705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="23" width="21.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="21" width="12.5450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
@@ -3527,9 +4025,12 @@
         <v>55</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3550,7 +4051,7 @@
       </c>
       <c r="E2" s="27" t="n">
         <f aca="false">SUMIF('tareas-ciclo1'!H4:H27,A2,'tareas-ciclo1'!G4:G27)</f>
-        <v>0.217522658610272</v>
+        <v>0.351219512195122</v>
       </c>
       <c r="F2" s="27" t="inlineStr">
         <f aca="false">E2</f>
@@ -3558,12 +4059,16 @@
           <t/>
         </is>
       </c>
-      <c r="G2" s="27" t="n">
+      <c r="G2" s="33" t="n">
+        <f aca="false">SUMIF('tareas-ciclo1'!R4:R27,A2,'tareas-ciclo1'!P4:P27)</f>
+        <v>19.5166666666667</v>
+      </c>
+      <c r="H2" s="27" t="n">
         <f aca="false">SUMIF('tareas-ciclo1'!R4:R27,A2,'tareas-ciclo1'!Q4:Q27)</f>
-        <v>0.0936555891238671</v>
-      </c>
-      <c r="H2" s="27" t="inlineStr">
-        <f aca="false">G2</f>
+        <v>0.151219512195122</v>
+      </c>
+      <c r="I2" s="27" t="inlineStr">
+        <f aca="false">H2</f>
         <is>
           <t/>
         </is>
@@ -3589,7 +4094,7 @@
       </c>
       <c r="E3" s="27" t="n">
         <f aca="false">SUMIF('tareas-ciclo1'!H4:H27,A3,'tareas-ciclo1'!G4:G27)</f>
-        <v>0.202416918429003</v>
+        <v>0.326829268292683</v>
       </c>
       <c r="F3" s="27" t="inlineStr">
         <f aca="false">E3+F2</f>
@@ -3597,12 +4102,16 @@
           <t/>
         </is>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="33" t="n">
+        <f aca="false">SUMIF('tareas-ciclo1'!R4:R27,A3,'tareas-ciclo1'!P4:P27)</f>
+        <v>15.1166666666667</v>
+      </c>
+      <c r="H3" s="27" t="n">
         <f aca="false">SUMIF('tareas-ciclo1'!R4:R27,A3,'tareas-ciclo1'!Q4:Q27)</f>
-        <v>0.081570996978852</v>
-      </c>
-      <c r="H3" s="27" t="inlineStr">
-        <f aca="false">G3+H2</f>
+        <v>0.131707317073171</v>
+      </c>
+      <c r="I3" s="27" t="inlineStr">
+        <f aca="false">H3+I2</f>
         <is>
           <t/>
         </is>
@@ -3628,7 +4137,7 @@
       </c>
       <c r="E4" s="27" t="n">
         <f aca="false">SUMIF('tareas-ciclo1'!H4:H27,A4,'tareas-ciclo1'!G4:G27)</f>
-        <v>0.199395770392749</v>
+        <v>0.321951219512195</v>
       </c>
       <c r="F4" s="27" t="inlineStr">
         <f aca="false">E4+F3</f>
@@ -3636,15 +4145,40 @@
           <t/>
         </is>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="33" t="n">
+        <f aca="false">SUMIF('tareas-ciclo1'!R4:R27,A4,'tareas-ciclo1'!P4:P27)</f>
+        <v>39.8833333333333</v>
+      </c>
+      <c r="H4" s="27" t="n">
         <f aca="false">SUMIF('tareas-ciclo1'!R4:R27,A4,'tareas-ciclo1'!Q4:Q27)</f>
-        <v>0.217522658610272</v>
-      </c>
-      <c r="H4" s="27" t="inlineStr">
-        <f aca="false">G4+H3</f>
+        <v>0.351219512195122</v>
+      </c>
+      <c r="I4" s="27" t="inlineStr">
+        <f aca="false">H4+I3</f>
         <is>
           <t/>
         </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
+      <c r="C5" s="0"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
+      <c r="A6" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="21" t="n">
+        <f aca="false">SUM(C2:C4)</f>
+        <v>105</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <f aca="false">SUM(D2:D4)</f>
+        <v>102.5</v>
+      </c>
+      <c r="G6" s="34" t="n">
+        <f aca="false">SUM(G2:G4)</f>
+        <v>74.5166666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de las gráficas del plan.
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -454,7 +454,7 @@
     <numFmt formatCode="0.00%" numFmtId="165"/>
     <numFmt formatCode="MM/DD/YYYY" numFmtId="166"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -499,18 +499,13 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <sz val="13"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="13"/>
     </font>
   </fonts>
   <fills count="4">
@@ -574,7 +569,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -621,6 +616,9 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
@@ -636,7 +634,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
@@ -648,24 +646,13 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0">
@@ -690,7 +677,7 @@
       <rgbColor rgb="00FFFF00"/>
       <rgbColor rgb="00FF00FF"/>
       <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="007E0021"/>
       <rgbColor rgb="00008000"/>
       <rgbColor rgb="00000080"/>
       <rgbColor rgb="00808000"/>
@@ -714,7 +701,7 @@
       <rgbColor rgb="00800000"/>
       <rgbColor rgb="00008080"/>
       <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="0000B8FF"/>
       <rgbColor rgb="00CCFFFF"/>
       <rgbColor rgb="00CCFFCC"/>
       <rgbColor rgb="00FFFF99"/>
@@ -731,7 +718,7 @@
       <rgbColor rgb="00666699"/>
       <rgbColor rgb="00969696"/>
       <rgbColor rgb="00004586"/>
-      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00579D1C"/>
       <rgbColor rgb="00003300"/>
       <rgbColor rgb="00333300"/>
       <rgbColor rgb="00993300"/>
@@ -743,7 +730,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart155.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -758,7 +745,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Ganancias Estimadas vs Ganancias Obtenidas</a:t>
             </a:r>
           </a:p>
@@ -990,11 +977,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="48913181"/>
-        <c:axId val="15193612"/>
+        <c:axId val="58807470"/>
+        <c:axId val="9345397"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48913181"/>
+        <c:axId val="58807470"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,8 +989,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15193612"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9345397"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1016,7 +1003,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15193612"/>
+        <c:axId val="9345397"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,8 +1020,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48913181"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="58807470"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -1065,7 +1052,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart156.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1080,7 +1067,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Horas Disponibles vs Horas Estimadas vs Horas Trabajadas</a:t>
             </a:r>
           </a:p>
@@ -1402,11 +1389,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="15400964"/>
-        <c:axId val="72341899"/>
+        <c:axId val="14217580"/>
+        <c:axId val="20667980"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="15400964"/>
+        <c:axId val="14217580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,8 +1401,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72341899"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="20667980"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1428,7 +1415,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72341899"/>
+        <c:axId val="20667980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,8 +1432,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15400964"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="14217580"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -1477,7 +1464,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart157.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1621,18 +1608,18 @@
                   <c:v>0.374358974358974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.743589743589744</c:v>
+                  <c:v>0.743589743589743</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="2890276"/>
-        <c:axId val="70533176"/>
+        <c:axId val="90399656"/>
+        <c:axId val="67441229"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2890276"/>
+        <c:axId val="90399656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70533176"/>
+        <c:crossAx val="67441229"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1654,7 +1641,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70533176"/>
+        <c:axId val="67441229"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2890276"/>
+        <c:crossAx val="90399656"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1703,7 +1690,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart158.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1847,11 +1834,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="31790695"/>
-        <c:axId val="28589913"/>
+        <c:axId val="12858955"/>
+        <c:axId val="97040498"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31790695"/>
+        <c:axId val="12858955"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +1846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="28589913"/>
+        <c:crossAx val="97040498"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1873,7 +1860,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28589913"/>
+        <c:axId val="97040498"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31790695"/>
+        <c:crossAx val="12858955"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1922,7 +1909,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart159.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1937,7 +1924,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Team Leader</a:t>
             </a:r>
           </a:p>
@@ -2060,11 +2047,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="23603586"/>
-        <c:axId val="50725992"/>
+        <c:axId val="9831491"/>
+        <c:axId val="38958556"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23603586"/>
+        <c:axId val="9831491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,8 +2059,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50725992"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="38958556"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2086,7 +2073,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50725992"/>
+        <c:axId val="38958556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,8 +2090,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="23603586"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9831491"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2135,7 +2122,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart160.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2150,7 +2137,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Development Manager</a:t>
             </a:r>
           </a:p>
@@ -2273,11 +2260,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="14111205"/>
-        <c:axId val="3823844"/>
+        <c:axId val="55636552"/>
+        <c:axId val="96718647"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14111205"/>
+        <c:axId val="55636552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2285,8 +2272,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3823844"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="96718647"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2299,7 +2286,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3823844"/>
+        <c:axId val="96718647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2316,8 +2303,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="14111205"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="55636552"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2348,7 +2335,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart161.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2363,7 +2350,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Process/Quality Manager</a:t>
             </a:r>
           </a:p>
@@ -2452,11 +2439,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="9283474"/>
-        <c:axId val="84767138"/>
+        <c:axId val="54964556"/>
+        <c:axId val="82855311"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="9283474"/>
+        <c:axId val="54964556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2464,8 +2451,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84767138"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="82855311"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2478,7 +2465,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84767138"/>
+        <c:axId val="82855311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,8 +2482,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9283474"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="54964556"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2527,7 +2514,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart162.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2542,7 +2529,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Planning Manager</a:t>
             </a:r>
           </a:p>
@@ -2665,11 +2652,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="71839073"/>
-        <c:axId val="38165250"/>
+        <c:axId val="42665869"/>
+        <c:axId val="53620963"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71839073"/>
+        <c:axId val="42665869"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,8 +2664,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38165250"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="53620963"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2691,7 +2678,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38165250"/>
+        <c:axId val="53620963"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2708,8 +2695,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71839073"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="42665869"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2740,7 +2727,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart163.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2755,7 +2742,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Support Manager</a:t>
             </a:r>
           </a:p>
@@ -2878,11 +2865,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="97629270"/>
-        <c:axId val="67564194"/>
+        <c:axId val="50658730"/>
+        <c:axId val="64270945"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97629270"/>
+        <c:axId val="50658730"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,8 +2877,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67564194"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="64270945"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2904,7 +2891,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67564194"/>
+        <c:axId val="64270945"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2921,8 +2908,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97629270"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="50658730"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2953,7 +2940,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart164.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2968,7 +2955,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Horas Estimadas vs Horas Trabajadas</a:t>
             </a:r>
           </a:p>
@@ -3091,11 +3078,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="48242007"/>
-        <c:axId val="65681085"/>
+        <c:axId val="34601567"/>
+        <c:axId val="42590453"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48242007"/>
+        <c:axId val="34601567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,8 +3090,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65681085"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="42590453"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -3117,7 +3104,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65681085"/>
+        <c:axId val="42590453"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,7 +3121,367 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48242007"/>
+        <c:crossAx val="34601567"/>
+        <c:crossesAt val="0"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:spPr/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Trabajadas Team Leader</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tiempo-ciclo1'!$I$2:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Trabajadas Development Manager</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tiempo-ciclo1'!$J$2:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Trabajadas Process/Quality Manager</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tiempo-ciclo1'!$K$2:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Trabajadas Planning Manager</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tiempo-ciclo1'!$L$2:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Trabajadas Support Manager</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00b8ff"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tiempo-ciclo1'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tiempo-ciclo1'!$M$2:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="25199999"/>
+        <c:axId val="77744924"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="25199999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77744924"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77744924"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="25199999"/>
         <c:crosses val="autoZero"/>
         <c:spPr>
           <a:ln>
@@ -3171,15 +3518,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>222120</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:colOff>249120</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>202320</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:colOff>228960</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3187,8 +3534,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="222120" y="3197880"/>
-        <a:ext cx="10734480" cy="3241800"/>
+        <a:off x="249120" y="2667960"/>
+        <a:ext cx="10788120" cy="3024360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3201,15 +3548,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>296280</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:colOff>323280</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>234000</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:colOff>260640</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3217,8 +3564,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="296280" y="7170840"/>
-        <a:ext cx="10692000" cy="3711240"/>
+        <a:off x="323280" y="6363720"/>
+        <a:ext cx="10745640" cy="3457440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3236,15 +3583,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:colOff>228960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>494640</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:colOff>479160</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3252,8 +3599,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="244080" y="1700640"/>
-        <a:ext cx="8004960" cy="2807280"/>
+        <a:off x="228960" y="1508400"/>
+        <a:ext cx="8043480" cy="2613960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3266,15 +3613,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:colOff>287640</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>442800</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:colOff>469440</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3282,8 +3629,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="260640" y="4872960"/>
-        <a:ext cx="7936560" cy="2806920"/>
+        <a:off x="287640" y="4222800"/>
+        <a:ext cx="7975080" cy="2613240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3301,15 +3648,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:colOff>280440</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>814680</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:colOff>841320</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3317,8 +3664,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="253440" y="2251080"/>
-        <a:ext cx="5762880" cy="3241080"/>
+        <a:off x="280440" y="1635120"/>
+        <a:ext cx="5789160" cy="3023280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3331,15 +3678,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>358920</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>385920</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>920160</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:colOff>946800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3347,8 +3694,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="358920" y="5731560"/>
-        <a:ext cx="5762880" cy="3240720"/>
+        <a:off x="385920" y="4874040"/>
+        <a:ext cx="5789160" cy="3023280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3361,15 +3708,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>353880</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:colOff>380880</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>911880</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:colOff>938520</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3377,8 +3724,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="353880" y="9296280"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="380880" y="8197560"/>
+        <a:ext cx="5785920" cy="3022200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3391,15 +3738,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>388800</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>54720</xdr:rowOff>
+      <xdr:colOff>415800</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>946800</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:colOff>973440</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3407,8 +3754,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="388800" y="12939480"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="415800" y="11587320"/>
+        <a:ext cx="5785920" cy="3022200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3421,15 +3768,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>431640</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:colOff>458640</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>989640</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:colOff>1016280</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3437,8 +3784,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="431640" y="16583760"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="458640" y="14978520"/>
+        <a:ext cx="5785920" cy="3022200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3451,15 +3798,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>155520</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:colOff>182520</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:colOff>272520</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3467,12 +3814,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7551720" y="2204280"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="7616880" y="1600560"/>
+        <a:ext cx="5788440" cy="3009600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>61920</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>306720</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>59760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7679880" y="5002920"/>
+        <a:ext cx="5759640" cy="3236760"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3489,21 +3866,20 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.56470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="40.4627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.60392156862745"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.6156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="21.6156862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="1023" min="12" style="4" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.58039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="40.6627450980392"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.0470588235294"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.6156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.7254901960784"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="21.7254901960784"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.0470588235294"/>
+    <col collapsed="false" hidden="false" max="1023" min="12" style="4" width="12.0470588235294"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -3589,7 +3965,7 @@
       </c>
       <c r="I3" s="1" t="n">
         <f aca="false">'tareas-ciclo1'!O4</f>
-        <v>4.46666666666667</v>
+        <v>4.46666666666666</v>
       </c>
       <c r="J3" s="3" t="inlineStr">
         <f aca="false">F3</f>
@@ -3597,9 +3973,11 @@
           <t/>
         </is>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="16" t="inlineStr">
         <f aca="false">'tareas-ciclo1'!Q4</f>
-        <v>1</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="4">
@@ -3627,7 +4005,7 @@
       </c>
       <c r="I4" s="1" t="n">
         <f aca="false">'tareas-ciclo1'!O5</f>
-        <v>5.08333333333333</v>
+        <v>5.08333333333335</v>
       </c>
       <c r="J4" s="3" t="inlineStr">
         <f aca="false">F4</f>
@@ -3716,28 +4094,28 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7" s="20">
       <c r="A7" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="17" t="n">
+      <c r="E7" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F7" s="9" t="n">
         <f aca="false">E7/E1</f>
         <v>0.00302114803625378</v>
       </c>
-      <c r="G7" s="18" t="n">
+      <c r="G7" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="17" t="n">
+      <c r="I7" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O8</f>
         <v>0.25</v>
       </c>
@@ -3752,32 +4130,32 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="20">
       <c r="A8" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E8" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F8" s="9" t="n">
         <f aca="false">E8/E1</f>
         <v>0.00302114803625378</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G8" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="17" t="n">
+      <c r="I8" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O9</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="J8" s="20" t="inlineStr">
+      <c r="J8" s="21" t="inlineStr">
         <f aca="false">F8</f>
         <is>
           <t/>
@@ -3788,34 +4166,34 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="20">
       <c r="A9" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F9" s="9" t="n">
         <f aca="false">E9/E1</f>
         <v>0.00302114803625378</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="17" t="n">
+      <c r="I9" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O10</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="J9" s="20" t="inlineStr">
+      <c r="J9" s="21" t="inlineStr">
         <f aca="false">F9</f>
         <is>
           <t/>
@@ -3826,34 +4204,34 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="20">
       <c r="A10" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E10" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">E10/E1</f>
         <v>0.0120845921450151</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="17" t="n">
+      <c r="I10" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O11</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J10" s="20" t="inlineStr">
+      <c r="J10" s="21" t="inlineStr">
         <f aca="false">F10</f>
         <is>
           <t/>
@@ -3864,68 +4242,68 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="20">
       <c r="A11" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="17" t="n">
+      <c r="E11" s="18" t="n">
         <v>3</v>
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">E11/E1</f>
         <v>0.0181268882175227</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="17" t="n">
+      <c r="I11" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O12</f>
         <v>3.9</v>
       </c>
-      <c r="J11" s="20" t="inlineStr">
+      <c r="J11" s="21" t="inlineStr">
         <f aca="false">F11</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K11" s="17" t="n">
+      <c r="K11" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q12</f>
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="20">
       <c r="A12" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E12" s="18" t="n">
         <v>10</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">E12/E1</f>
         <v>0.0604229607250755</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="17" t="n">
+      <c r="I12" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O13</f>
         <v>0</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="17" t="n">
+      <c r="J12" s="21"/>
+      <c r="K12" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q13</f>
         <v>1</v>
       </c>
@@ -3934,10 +4312,10 @@
       <c r="A13" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="1" t="n">
@@ -3959,242 +4337,242 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="20">
       <c r="A14" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17" t="n">
+      <c r="D14" s="17"/>
+      <c r="E14" s="18" t="n">
         <v>10</v>
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">E14/E1</f>
         <v>0.0604229607250755</v>
       </c>
-      <c r="G14" s="17" t="n">
+      <c r="G14" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="17" t="n">
+      <c r="I14" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O15</f>
         <v>8</v>
       </c>
-      <c r="J14" s="20" t="inlineStr">
+      <c r="J14" s="21" t="inlineStr">
         <f aca="false">F14</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q15</f>
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="20">
       <c r="A15" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="17" t="n">
+      <c r="E15" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">E15/E1</f>
         <v>0.0120845921450151</v>
       </c>
-      <c r="G15" s="17" t="n">
+      <c r="G15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="17" t="n">
+      <c r="I15" s="19" t="n">
         <f aca="false">'tareas-ciclo1'!O16</f>
         <v>15.4166666666667</v>
       </c>
-      <c r="J15" s="20" t="inlineStr">
+      <c r="J15" s="22" t="inlineStr">
         <f aca="false">SUM(F15:F17)</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K15" s="21" t="n">
+      <c r="K15" s="19" t="n">
         <f aca="false">'tareas-ciclo1'!Q16</f>
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="20">
       <c r="A16" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="17" t="n">
+      <c r="E16" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">E16/E1</f>
         <v>0.0120845921450151</v>
       </c>
-      <c r="G16" s="17" t="n">
+      <c r="G16" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="17" s="19">
+      <c r="I16" s="19"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="17" s="20">
       <c r="A17" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E17" s="18" t="n">
         <v>4</v>
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">E17/E1</f>
         <v>0.0241691842900302</v>
       </c>
-      <c r="G17" s="17" t="n">
+      <c r="G17" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18" s="19">
+      <c r="I17" s="19"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18" s="20">
       <c r="A18" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="17" t="n">
+      <c r="E18" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">E18/E1</f>
         <v>0.00302114803625378</v>
       </c>
-      <c r="G18" s="17" t="n">
+      <c r="G18" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I18" s="17" t="n">
+      <c r="I18" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O19</f>
         <v>0.383333333333333</v>
       </c>
-      <c r="J18" s="20" t="inlineStr">
+      <c r="J18" s="21" t="inlineStr">
         <f aca="false">F18</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K18" s="17" t="n">
+      <c r="K18" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q19</f>
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="20">
       <c r="A19" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="17" t="n">
+      <c r="E19" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">E19/E1</f>
         <v>0.0120845921450151</v>
       </c>
-      <c r="G19" s="17" t="n">
+      <c r="G19" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="I19" s="17" t="n">
+      <c r="I19" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O20</f>
         <v>1</v>
       </c>
-      <c r="J19" s="20" t="inlineStr">
+      <c r="J19" s="21" t="inlineStr">
         <f aca="false">F19</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K19" s="17" t="n">
+      <c r="K19" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q20</f>
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="20">
       <c r="A20" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17" t="n">
+      <c r="D20" s="17"/>
+      <c r="E20" s="18" t="n">
         <v>10</v>
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">E20/E1</f>
         <v>0.0604229607250755</v>
       </c>
-      <c r="G20" s="17" t="n">
+      <c r="G20" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="I20" s="17" t="n">
+      <c r="I20" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O21</f>
-        <v>8.16666666666667</v>
-      </c>
-      <c r="J20" s="20" t="inlineStr">
+        <v>8.16666666666665</v>
+      </c>
+      <c r="J20" s="21" t="inlineStr">
         <f aca="false">F20</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K20" s="17" t="n">
+      <c r="K20" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q21</f>
         <v>3</v>
       </c>
@@ -4355,7 +4733,7 @@
       <c r="A25" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="17" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -4393,7 +4771,7 @@
       <c r="A26" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -4606,10 +4984,10 @@
       <c r="B35" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="17" t="s">
         <v>85</v>
       </c>
       <c r="E35" s="1" t="n">
@@ -4630,10 +5008,10 @@
       <c r="B36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="17" t="s">
         <v>88</v>
       </c>
       <c r="E36" s="1" t="n">
@@ -4678,7 +5056,7 @@
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="17" t="s">
         <v>93</v>
       </c>
       <c r="E38" s="1" t="n">
@@ -4853,24 +5231,24 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="I50" activeCellId="0" pane="topLeft" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="12.6705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="16.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="19.6627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="24" width="21.3607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="22" width="12.6705882352941"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.7607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="18.4941176470588"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="25" width="21.4705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="23" width="12.7333333333333"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -4896,25 +5274,25 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="26" t="n">
+      <c r="A2" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="28" t="n">
         <v>41902</v>
       </c>
-      <c r="C2" s="26" t="n">
+      <c r="C2" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D2" s="26" t="n">
+      <c r="D2" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A2,_gTDHE)</f>
         <v>36</v>
       </c>
-      <c r="E2" s="28" t="n">
+      <c r="E2" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A2,_gPIDGE)</f>
         <v>0.217522658610272</v>
       </c>
-      <c r="F2" s="28" t="inlineStr">
+      <c r="F2" s="29" t="inlineStr">
         <f aca="false">E2</f>
         <is>
           <t/>
@@ -4924,11 +5302,11 @@
         <f aca="false">SUMIF(_gSR,A2,_gTDHT)</f>
         <v>17.65</v>
       </c>
-      <c r="H2" s="28" t="n">
+      <c r="H2" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A2,_gPIDGO)</f>
         <v>0.138972809667674</v>
       </c>
-      <c r="I2" s="28" t="inlineStr">
+      <c r="I2" s="29" t="inlineStr">
         <f aca="false">H2</f>
         <is>
           <t/>
@@ -4936,28 +5314,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="26" t="n">
+      <c r="A3" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="inlineStr">
+      <c r="B3" s="28" t="inlineStr">
         <f aca="false">B2+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C3" s="26" t="n">
+      <c r="C3" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D3" s="26" t="n">
+      <c r="D3" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A3,_gTDHE)</f>
         <v>33.5</v>
       </c>
-      <c r="E3" s="28" t="n">
+      <c r="E3" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A3,_gPIDGE)</f>
         <v>0.202416918429003</v>
       </c>
-      <c r="F3" s="28" t="inlineStr">
+      <c r="F3" s="29" t="inlineStr">
         <f aca="false">E3+F2</f>
         <is>
           <t/>
@@ -4967,11 +5345,11 @@
         <f aca="false">SUMIF(_gSR,A3,_gTDHT)</f>
         <v>15.1166666666667</v>
       </c>
-      <c r="H3" s="28" t="n">
+      <c r="H3" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A3,_gPIDGO)</f>
         <v>0.081570996978852</v>
       </c>
-      <c r="I3" s="28" t="inlineStr">
+      <c r="I3" s="29" t="inlineStr">
         <f aca="false">H3+I2</f>
         <is>
           <t/>
@@ -4979,28 +5357,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="26" t="n">
+      <c r="A4" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="inlineStr">
+      <c r="B4" s="28" t="inlineStr">
         <f aca="false">B3+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C4" s="26" t="n">
+      <c r="C4" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D4" s="26" t="n">
+      <c r="D4" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A4,_gTDHE)</f>
         <v>28</v>
       </c>
-      <c r="E4" s="28" t="n">
+      <c r="E4" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A4,_gPIDGE)</f>
         <v>0.169184290030211</v>
       </c>
-      <c r="F4" s="28" t="inlineStr">
+      <c r="F4" s="29" t="inlineStr">
         <f aca="false">E4+F3</f>
         <is>
           <t/>
@@ -5010,11 +5388,11 @@
         <f aca="false">SUMIF(_gSR,A4,_gTDHT)</f>
         <v>39.8833333333333</v>
       </c>
-      <c r="H4" s="28" t="n">
+      <c r="H4" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A4,_gPIDGO)</f>
         <v>0.217522658610272</v>
       </c>
-      <c r="I4" s="28" t="inlineStr">
+      <c r="I4" s="29" t="inlineStr">
         <f aca="false">H4+I3</f>
         <is>
           <t/>
@@ -5022,28 +5400,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
-      <c r="A5" s="26" t="n">
+      <c r="A5" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="inlineStr">
+      <c r="B5" s="28" t="inlineStr">
         <f aca="false">B4+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C5" s="26" t="n">
+      <c r="C5" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D5" s="26" t="n">
+      <c r="D5" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A5,_gTDHE)</f>
         <v>42.5</v>
       </c>
-      <c r="E5" s="28" t="n">
+      <c r="E5" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A5,_gPIDGE)</f>
         <v>0.256797583081571</v>
       </c>
-      <c r="F5" s="28" t="inlineStr">
+      <c r="F5" s="29" t="inlineStr">
         <f aca="false">E5+F4</f>
         <is>
           <t/>
@@ -5053,11 +5431,11 @@
         <f aca="false">SUMIF(_gSR,A5,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="28" t="n">
+      <c r="H5" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A5,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="28" t="inlineStr">
+      <c r="I5" s="29" t="inlineStr">
         <f aca="false">H5+I4</f>
         <is>
           <t/>
@@ -5065,28 +5443,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="6">
-      <c r="A6" s="26" t="n">
+      <c r="A6" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="inlineStr">
+      <c r="B6" s="28" t="inlineStr">
         <f aca="false">B5+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C6" s="26" t="n">
+      <c r="C6" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D6" s="26" t="n">
+      <c r="D6" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A6,_gTDHE)</f>
         <v>25.5</v>
       </c>
-      <c r="E6" s="28" t="n">
+      <c r="E6" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A6,_gPIDGE)</f>
         <v>0.154078549848943</v>
       </c>
-      <c r="F6" s="28" t="inlineStr">
+      <c r="F6" s="29" t="inlineStr">
         <f aca="false">E6+F5</f>
         <is>
           <t/>
@@ -5096,11 +5474,11 @@
         <f aca="false">SUMIF(_gSR,A6,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="28" t="n">
+      <c r="H6" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A6,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="28" t="inlineStr">
+      <c r="I6" s="29" t="inlineStr">
         <f aca="false">H6+I5</f>
         <is>
           <t/>
@@ -5108,28 +5486,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="7">
-      <c r="A7" s="26" t="n">
+      <c r="A7" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="inlineStr">
+      <c r="B7" s="28" t="inlineStr">
         <f aca="false">B6+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C7" s="26" t="n">
+      <c r="C7" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D7" s="26" t="n">
+      <c r="D7" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A7,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="28" t="n">
+      <c r="E7" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A7,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="28" t="inlineStr">
+      <c r="F7" s="29" t="inlineStr">
         <f aca="false">E7+F6</f>
         <is>
           <t/>
@@ -5139,11 +5517,11 @@
         <f aca="false">SUMIF(_gSR,A7,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="28" t="n">
+      <c r="H7" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A7,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="28" t="inlineStr">
+      <c r="I7" s="29" t="inlineStr">
         <f aca="false">H7+I6</f>
         <is>
           <t/>
@@ -5151,28 +5529,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="8">
-      <c r="A8" s="26" t="n">
+      <c r="A8" s="27" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="inlineStr">
+      <c r="B8" s="28" t="inlineStr">
         <f aca="false">B7+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C8" s="26" t="n">
+      <c r="C8" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D8" s="26" t="n">
+      <c r="D8" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A8,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="28" t="n">
+      <c r="E8" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A8,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="28" t="inlineStr">
+      <c r="F8" s="29" t="inlineStr">
         <f aca="false">E8+F7</f>
         <is>
           <t/>
@@ -5182,11 +5560,11 @@
         <f aca="false">SUMIF(_gSR,A8,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="28" t="n">
+      <c r="H8" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A8,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="28" t="inlineStr">
+      <c r="I8" s="29" t="inlineStr">
         <f aca="false">H8+I7</f>
         <is>
           <t/>
@@ -5194,28 +5572,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="9">
-      <c r="A9" s="26" t="n">
+      <c r="A9" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="inlineStr">
+      <c r="B9" s="28" t="inlineStr">
         <f aca="false">B8+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C9" s="26" t="n">
+      <c r="C9" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D9" s="26" t="n">
+      <c r="D9" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A9,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="28" t="n">
+      <c r="E9" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A9,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="28" t="inlineStr">
+      <c r="F9" s="29" t="inlineStr">
         <f aca="false">E9+F8</f>
         <is>
           <t/>
@@ -5225,11 +5603,11 @@
         <f aca="false">SUMIF(_gSR,A9,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="28" t="n">
+      <c r="H9" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A9,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="28" t="inlineStr">
+      <c r="I9" s="29" t="inlineStr">
         <f aca="false">H9+I8</f>
         <is>
           <t/>
@@ -5237,28 +5615,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="10">
-      <c r="A10" s="26" t="n">
+      <c r="A10" s="27" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="inlineStr">
+      <c r="B10" s="28" t="inlineStr">
         <f aca="false">B9+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C10" s="26" t="n">
+      <c r="C10" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D10" s="26" t="n">
+      <c r="D10" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A10,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="28" t="n">
+      <c r="E10" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A10,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="28" t="inlineStr">
+      <c r="F10" s="29" t="inlineStr">
         <f aca="false">E10+F9</f>
         <is>
           <t/>
@@ -5268,11 +5646,11 @@
         <f aca="false">SUMIF(_gSR,A10,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="28" t="n">
+      <c r="H10" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A10,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="28" t="inlineStr">
+      <c r="I10" s="29" t="inlineStr">
         <f aca="false">H10+I9</f>
         <is>
           <t/>
@@ -5280,28 +5658,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="11">
-      <c r="A11" s="26" t="n">
+      <c r="A11" s="27" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="inlineStr">
+      <c r="B11" s="28" t="inlineStr">
         <f aca="false">B10+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C11" s="26" t="n">
+      <c r="C11" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D11" s="26" t="n">
+      <c r="D11" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A11,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="28" t="n">
+      <c r="E11" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A11,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="28" t="inlineStr">
+      <c r="F11" s="29" t="inlineStr">
         <f aca="false">E11+F10</f>
         <is>
           <t/>
@@ -5311,11 +5689,11 @@
         <f aca="false">SUMIF(_gSR,A11,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="28" t="n">
+      <c r="H11" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A11,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="28" t="inlineStr">
+      <c r="I11" s="29" t="inlineStr">
         <f aca="false">H11+I10</f>
         <is>
           <t/>
@@ -5323,28 +5701,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="12">
-      <c r="A12" s="26" t="n">
+      <c r="A12" s="27" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="inlineStr">
+      <c r="B12" s="28" t="inlineStr">
         <f aca="false">B11+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C12" s="26" t="n">
+      <c r="C12" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D12" s="26" t="n">
+      <c r="D12" s="27" t="n">
         <f aca="false">SUMIF(_gSE,A12,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="28" t="n">
+      <c r="E12" s="29" t="n">
         <f aca="false">SUMIF(_gSE,A12,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="28" t="inlineStr">
+      <c r="F12" s="29" t="inlineStr">
         <f aca="false">E12+F11</f>
         <is>
           <t/>
@@ -5354,32 +5732,34 @@
         <f aca="false">SUMIF(_gSR,A12,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="28" t="n">
+      <c r="H12" s="29" t="n">
         <f aca="false">SUMIF(_gSR,A12,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="28" t="inlineStr">
+      <c r="I12" s="29" t="inlineStr">
         <f aca="false">H12+I11</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="14">
       <c r="A14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="22" t="n">
+      <c r="C14" s="23" t="n">
         <f aca="false">SUM(C2:C12)</f>
         <v>385</v>
       </c>
-      <c r="D14" s="22" t="n">
+      <c r="D14" s="23" t="n">
         <f aca="false">SUM(D2:D12)</f>
         <v>165.5</v>
       </c>
-      <c r="G14" s="30" t="n">
+      <c r="G14" s="25" t="inlineStr">
         <f aca="false">SUM(G2:G12)</f>
-        <v>72.65</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -5401,25 +5781,24 @@
   </sheetPr>
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="F19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M4" activeCellId="0" pane="topLeft" sqref="M4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L27" activeCellId="0" pane="topLeft" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.58039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="40.4627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.71372549019608"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="20.2313725490196"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="2.71372549019608"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="4" width="2.71372549019608"/>
-    <col collapsed="false" hidden="false" max="23" min="19" style="4" width="20.2313725490196"/>
-    <col collapsed="false" hidden="false" max="1023" min="24" style="4" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.6"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="40.6627450980392"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.0470588235294"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.73333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="20.3333333333333"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="2.73333333333333"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.0470588235294"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="4" width="2.73333333333333"/>
+    <col collapsed="false" hidden="false" max="23" min="19" style="4" width="20.3333333333333"/>
+    <col collapsed="false" hidden="false" max="1023" min="24" style="4" width="12.0470588235294"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -5455,7 +5834,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="31" t="n">
+      <c r="E2" s="30" t="n">
         <f aca="false">SUM(E4:E26)</f>
         <v>97.5</v>
       </c>
@@ -5618,15 +5997,15 @@
       </c>
       <c r="O4" s="1" t="n">
         <f aca="false">SUM(S4:W4)</f>
-        <v>4.46666666666667</v>
-      </c>
-      <c r="P4" s="32" t="inlineStr">
+        <v>4.46666666666666</v>
+      </c>
+      <c r="P4" s="3" t="inlineStr">
         <f aca="false">F4</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q4" s="32" t="n">
+      <c r="Q4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="R4" s="1"/>
@@ -5688,7 +6067,7 @@
       </c>
       <c r="O5" s="1" t="n">
         <f aca="false">SUM(S5:W5)</f>
-        <v>5.08333333333333</v>
+        <v>5.08333333333335</v>
       </c>
       <c r="P5" s="3" t="inlineStr">
         <f aca="false">F5</f>
@@ -5843,34 +6222,34 @@
       </c>
       <c r="W7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="20">
       <c r="A8" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E8" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F8" s="9" t="n">
         <f aca="false">E8/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G8" s="18" t="n">
+      <c r="G8" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="17"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="18"/>
       <c r="O8" s="1" t="n">
         <f aca="false">SUM(S8:W8)</f>
         <v>0.25</v>
@@ -5881,47 +6260,47 @@
           <t/>
         </is>
       </c>
-      <c r="Q8" s="17" t="n">
+      <c r="Q8" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17" t="n">
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18" t="n">
         <f aca="false">15/60</f>
         <v>0.25</v>
       </c>
-      <c r="W8" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="19">
+      <c r="W8" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="20">
       <c r="A9" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F9" s="9" t="n">
         <f aca="false">E9/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M9" s="17"/>
+      <c r="M9" s="18"/>
       <c r="O9" s="1" t="n">
         <f aca="false">SUM(S9:W9)</f>
         <v>0.666666666666667</v>
@@ -5932,49 +6311,49 @@
           <t/>
         </is>
       </c>
-      <c r="Q9" s="17" t="n">
+      <c r="Q9" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17" t="n">
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="W9" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="19">
+      <c r="W9" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="20">
       <c r="A10" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E10" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">E10/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M10" s="17"/>
+      <c r="M10" s="18"/>
       <c r="O10" s="1" t="n">
         <f aca="false">SUM(S10:W10)</f>
         <v>0.416666666666667</v>
@@ -5985,51 +6364,51 @@
           <t/>
         </is>
       </c>
-      <c r="Q10" s="17" t="n">
+      <c r="Q10" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17" t="n">
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18" t="n">
         <f aca="false">25/60</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="W10" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="19">
+      <c r="W10" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="20">
       <c r="A11" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="17" t="n">
+      <c r="E11" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">E11/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="17" t="n">
+      <c r="I11" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="18"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="17" t="n">
+      <c r="L11" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="17"/>
+      <c r="M11" s="18"/>
       <c r="O11" s="1" t="n">
         <f aca="false">SUM(S11:W11)</f>
         <v>1.16666666666667</v>
@@ -6040,52 +6419,52 @@
           <t/>
         </is>
       </c>
-      <c r="Q11" s="17" t="n">
+      <c r="Q11" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17" t="n">
+      <c r="R11" s="18"/>
+      <c r="S11" s="18" t="n">
         <f aca="false">35/60</f>
         <v>0.583333333333333</v>
       </c>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17" t="n">
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18" t="n">
         <f aca="false">35/60</f>
         <v>0.583333333333333</v>
       </c>
-      <c r="W11" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="19">
+      <c r="W11" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="20">
       <c r="A12" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E12" s="18" t="n">
         <v>3</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">E12/E2</f>
         <v>0.0307692307692308</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17" t="n">
+      <c r="I12" s="18"/>
+      <c r="J12" s="18" t="n">
         <v>1.5</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17" t="n">
+      <c r="K12" s="18"/>
+      <c r="L12" s="18" t="n">
         <v>1.5</v>
       </c>
-      <c r="M12" s="17"/>
+      <c r="M12" s="18"/>
       <c r="O12" s="1" t="n">
         <f aca="false">SUM(S12:W12)</f>
         <v>3.9</v>
@@ -6096,71 +6475,71 @@
           <t/>
         </is>
       </c>
-      <c r="Q12" s="17" t="n">
+      <c r="Q12" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17" t="n">
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18" t="n">
         <f aca="false">(45+72)/60</f>
         <v>1.95</v>
       </c>
-      <c r="U12" s="17"/>
-      <c r="V12" s="17" t="n">
+      <c r="U12" s="18"/>
+      <c r="V12" s="18" t="n">
         <f aca="false">(45+72)/60</f>
         <v>1.95</v>
       </c>
-      <c r="W12" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13" s="19">
+      <c r="W12" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13" s="20">
       <c r="A13" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="17" t="n">
+      <c r="E13" s="18" t="n">
         <v>10</v>
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">E13/E2</f>
         <v>0.102564102564103</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="17" t="n">
+      <c r="I13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="J13" s="17" t="n">
+      <c r="J13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="K13" s="17" t="n">
+      <c r="K13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="L13" s="17" t="n">
+      <c r="L13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="M13" s="17" t="n">
+      <c r="M13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="O13" s="33" t="n">
+      <c r="O13" s="31" t="n">
         <f aca="false">SUM(S13:W13)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34" t="n">
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
-      <c r="W13" s="17"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14">
       <c r="A14" s="14" t="n">
@@ -6169,7 +6548,7 @@
       <c r="B14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="1" t="n">
@@ -6197,12 +6576,12 @@
       <c r="M14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="O14" s="33" t="n">
+      <c r="O14" s="31" t="n">
         <f aca="false">SUM(S14:W14)</f>
         <v>2.83333333333333</v>
       </c>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33" t="n">
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31" t="n">
         <v>2</v>
       </c>
       <c r="R14" s="1"/>
@@ -6218,403 +6597,403 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="20">
       <c r="A15" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17" t="n">
+      <c r="D15" s="17"/>
+      <c r="E15" s="18" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">E15/E2</f>
         <v>0.102564102564103</v>
       </c>
-      <c r="G15" s="17" t="n">
+      <c r="G15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="17" t="n">
+      <c r="I15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="J15" s="17" t="n">
+      <c r="J15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="L15" s="17" t="n">
+      <c r="L15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="M15" s="17" t="n">
+      <c r="M15" s="18" t="n">
         <v>2</v>
       </c>
       <c r="O15" s="1" t="n">
         <f aca="false">SUM(S15:W15)</f>
         <v>8</v>
       </c>
-      <c r="P15" s="20" t="inlineStr">
+      <c r="P15" s="21" t="inlineStr">
         <f aca="false">F15</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q15" s="17" t="n">
+      <c r="Q15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17" t="n">
+      <c r="R15" s="18"/>
+      <c r="S15" s="18" t="n">
         <f aca="false">120/60</f>
         <v>2</v>
       </c>
-      <c r="T15" s="17" t="n">
+      <c r="T15" s="18" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
-      <c r="U15" s="17" t="n">
+      <c r="U15" s="18" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
-      <c r="V15" s="17" t="n">
+      <c r="V15" s="18" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
-      <c r="W15" s="17" t="n">
+      <c r="W15" s="18" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="20">
       <c r="A16" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="17" t="n">
+      <c r="E16" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">E16/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G16" s="17" t="n">
+      <c r="G16" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17" t="n">
+      <c r="I16" s="18"/>
+      <c r="J16" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17" t="n">
+      <c r="K16" s="18"/>
+      <c r="L16" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="M16" s="17"/>
+      <c r="M16" s="18"/>
       <c r="O16" s="14" t="n">
         <f aca="false">SUM(S16:W16)</f>
         <v>15.4166666666667</v>
       </c>
-      <c r="P16" s="35" t="inlineStr">
+      <c r="P16" s="22" t="inlineStr">
         <f aca="false">SUM(F16:F18)</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q16" s="36" t="n">
+      <c r="Q16" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="R16" s="17"/>
-      <c r="S16" s="18" t="n">
+      <c r="R16" s="18"/>
+      <c r="S16" s="19" t="n">
         <f aca="false">(40+75+90)/60</f>
         <v>3.41666666666667</v>
       </c>
-      <c r="T16" s="18" t="n">
+      <c r="T16" s="19" t="n">
         <f aca="false">(75+45+140)/60</f>
         <v>4.33333333333333</v>
       </c>
-      <c r="U16" s="18" t="n">
+      <c r="U16" s="19" t="n">
         <f aca="false">(120+50)/60</f>
         <v>2.83333333333333</v>
       </c>
-      <c r="V16" s="18" t="n">
+      <c r="V16" s="19" t="n">
         <f aca="false">75/60</f>
         <v>1.25</v>
       </c>
-      <c r="W16" s="18" t="n">
+      <c r="W16" s="19" t="n">
         <f aca="false">(140+75)/60</f>
         <v>3.58333333333333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="17" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="17" s="20">
       <c r="A17" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E17" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">E17/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G17" s="17" t="n">
+      <c r="G17" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17" t="n">
+      <c r="I17" s="18"/>
+      <c r="J17" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="18" s="19">
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="18" s="20">
       <c r="A18" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="17" t="n">
+      <c r="E18" s="18" t="n">
         <v>4</v>
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">E18/E2</f>
         <v>0.041025641025641</v>
       </c>
-      <c r="G18" s="17" t="n">
+      <c r="G18" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17" t="n">
+      <c r="I18" s="18"/>
+      <c r="J18" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="K18" s="17" t="n">
+      <c r="K18" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
       <c r="O18" s="14"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="19">
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="20">
       <c r="A19" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="17" t="n">
+      <c r="E19" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">E19/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G19" s="17" t="n">
+      <c r="G19" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="L19" s="17" t="n">
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="L19" s="18" t="n">
         <v>0.5</v>
       </c>
-      <c r="M19" s="17"/>
+      <c r="M19" s="18"/>
       <c r="O19" s="1" t="n">
         <f aca="false">SUM(S19:W19)</f>
         <v>0.383333333333333</v>
       </c>
-      <c r="P19" s="20" t="inlineStr">
+      <c r="P19" s="21" t="inlineStr">
         <f aca="false">F19</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q19" s="17" t="n">
+      <c r="Q19" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-      <c r="V19" s="17" t="n">
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="18" t="n">
         <f aca="false">23/60</f>
         <v>0.383333333333333</v>
       </c>
-      <c r="W19" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="19">
+      <c r="W19" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="20">
       <c r="A20" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="17" t="n">
+      <c r="E20" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">E20/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G20" s="17" t="n">
+      <c r="G20" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="I20" s="17" t="n">
+      <c r="I20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17" t="n">
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="1" t="n">
         <f aca="false">SUM(S20:W20)</f>
         <v>1</v>
       </c>
-      <c r="P20" s="20" t="inlineStr">
+      <c r="P20" s="21" t="inlineStr">
         <f aca="false">F20</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q20" s="17" t="n">
+      <c r="Q20" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17" t="n">
+      <c r="R20" s="18"/>
+      <c r="S20" s="18" t="n">
         <f aca="false">30/60</f>
         <v>0.5</v>
       </c>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-      <c r="W20" s="17" t="n">
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="18" t="n">
         <f aca="false">30/60</f>
         <v>0.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="21" s="19">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="21" s="20">
       <c r="A21" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17" t="n">
+      <c r="D21" s="17"/>
+      <c r="E21" s="18" t="n">
         <v>10</v>
       </c>
       <c r="F21" s="9" t="n">
         <f aca="false">E21/E2</f>
         <v>0.102564102564103</v>
       </c>
-      <c r="G21" s="17" t="n">
+      <c r="G21" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="I21" s="17" t="n">
+      <c r="I21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="J21" s="17" t="n">
+      <c r="J21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="K21" s="17" t="n">
+      <c r="K21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="L21" s="17" t="n">
+      <c r="L21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="M21" s="17" t="n">
+      <c r="M21" s="18" t="n">
         <v>2</v>
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">SUM(S21:W21)</f>
-        <v>8.16666666666667</v>
-      </c>
-      <c r="P21" s="20" t="inlineStr">
+        <v>8.16666666666665</v>
+      </c>
+      <c r="P21" s="21" t="inlineStr">
         <f aca="false">F21</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q21" s="17" t="n">
+      <c r="Q21" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17" t="n">
+      <c r="R21" s="18"/>
+      <c r="S21" s="18" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="T21" s="17" t="n">
+      <c r="T21" s="18" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="U21" s="17" t="n">
+      <c r="U21" s="18" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="V21" s="17" t="n">
+      <c r="V21" s="18" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="W21" s="17" t="n">
+      <c r="W21" s="18" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
@@ -6649,7 +7028,7 @@
         <f aca="false">SUM(S22:W22)</f>
         <v>2.5</v>
       </c>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <f aca="false">F22</f>
         <is>
           <t/>
@@ -6713,7 +7092,7 @@
         <f aca="false">SUM(S23:W23)</f>
         <v>6.25</v>
       </c>
-      <c r="P23" s="20" t="inlineStr">
+      <c r="P23" s="21" t="inlineStr">
         <f aca="false">F23</f>
         <is>
           <t/>
@@ -6777,7 +7156,7 @@
         <f aca="false">SUM(S24:W24)</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="P24" s="20" t="inlineStr">
+      <c r="P24" s="21" t="inlineStr">
         <f aca="false">F24</f>
         <is>
           <t/>
@@ -6832,7 +7211,7 @@
         <f aca="false">SUM(S25:W25)</f>
         <v>1.25</v>
       </c>
-      <c r="P25" s="20" t="inlineStr">
+      <c r="P25" s="21" t="inlineStr">
         <f aca="false">F25</f>
         <is>
           <t/>
@@ -6855,7 +7234,7 @@
       <c r="A26" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -6893,7 +7272,7 @@
         <f aca="false">SUM(S26:W26)</f>
         <v>3.66666666666667</v>
       </c>
-      <c r="P26" s="20" t="inlineStr">
+      <c r="P26" s="21" t="inlineStr">
         <f aca="false">F26</f>
         <is>
           <t/>
@@ -6955,26 +7334,26 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I6" activeCellId="0" pane="topLeft" sqref="I6"/>
+      <selection activeCell="I16" activeCellId="0" pane="topLeft" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="12.6705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="16.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="19.6627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="24" width="21.3607843137255"/>
-    <col collapsed="false" hidden="true" max="7" min="7" style="24" width="0"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="24" width="21.3607843137255"/>
-    <col collapsed="false" hidden="false" max="1014" min="10" style="22" width="12.6705882352941"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="12.6705882352941"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.7607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="18.4941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="25" width="21.4705882352941"/>
+    <col collapsed="false" hidden="true" max="7" min="7" style="25" width="0"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="25" width="21.4705882352941"/>
+    <col collapsed="false" hidden="false" max="1014" min="10" style="23" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="12.7333333333333"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -7000,25 +7379,25 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="26" t="n">
+      <c r="A2" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="28" t="n">
         <v>41902</v>
       </c>
-      <c r="C2" s="26" t="n">
+      <c r="C2" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D2" s="26" t="n">
+      <c r="D2" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1TDHE)</f>
         <v>36</v>
       </c>
-      <c r="E2" s="28" t="n">
+      <c r="E2" s="29" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1PIDGE)</f>
         <v>0.369230769230769</v>
       </c>
-      <c r="F2" s="28" t="inlineStr">
+      <c r="F2" s="29" t="inlineStr">
         <f aca="false">E2</f>
         <is>
           <t/>
@@ -7028,11 +7407,11 @@
         <f aca="false">SUMIF(_1SR,A2,_1TDHT)</f>
         <v>17.65</v>
       </c>
-      <c r="H2" s="28" t="n">
+      <c r="H2" s="29" t="n">
         <f aca="false">SUMIF(_1SR,A2,_1PIDGO)</f>
         <v>0.235897435897436</v>
       </c>
-      <c r="I2" s="28" t="inlineStr">
+      <c r="I2" s="29" t="inlineStr">
         <f aca="false">H2</f>
         <is>
           <t/>
@@ -7040,28 +7419,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="26" t="n">
+      <c r="A3" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="inlineStr">
+      <c r="B3" s="28" t="inlineStr">
         <f aca="false">B2+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C3" s="26" t="n">
+      <c r="C3" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D3" s="26" t="n">
+      <c r="D3" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1TDHE)</f>
         <v>33.5</v>
       </c>
-      <c r="E3" s="28" t="n">
+      <c r="E3" s="29" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1PIDGE)</f>
         <v>0.343589743589744</v>
       </c>
-      <c r="F3" s="28" t="inlineStr">
+      <c r="F3" s="29" t="inlineStr">
         <f aca="false">E3+F2</f>
         <is>
           <t/>
@@ -7071,11 +7450,11 @@
         <f aca="false">SUMIF(_1SR,A3,_1TDHT)</f>
         <v>15.1166666666667</v>
       </c>
-      <c r="H3" s="28" t="n">
+      <c r="H3" s="29" t="n">
         <f aca="false">SUMIF(_1SR,A3,_1PIDGO)</f>
-        <v>0.138461538461538</v>
-      </c>
-      <c r="I3" s="28" t="inlineStr">
+        <v>0.138461538461539</v>
+      </c>
+      <c r="I3" s="29" t="inlineStr">
         <f aca="false">H3+I2</f>
         <is>
           <t/>
@@ -7083,28 +7462,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="26" t="n">
+      <c r="A4" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="inlineStr">
+      <c r="B4" s="28" t="inlineStr">
         <f aca="false">B3+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C4" s="26" t="n">
+      <c r="C4" s="27" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D4" s="26" t="n">
+      <c r="D4" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1TDHE)</f>
         <v>28</v>
       </c>
-      <c r="E4" s="28" t="n">
+      <c r="E4" s="29" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1PIDGE)</f>
         <v>0.287179487179487</v>
       </c>
-      <c r="F4" s="28" t="inlineStr">
+      <c r="F4" s="29" t="inlineStr">
         <f aca="false">E4+F3</f>
         <is>
           <t/>
@@ -7114,35 +7493,34 @@
         <f aca="false">SUMIF(_1SR,A4,_1TDHT)</f>
         <v>39.8833333333333</v>
       </c>
-      <c r="H4" s="28" t="n">
+      <c r="H4" s="29" t="n">
         <f aca="false">SUMIF(_1SR,A4,_1PIDGO)</f>
-        <v>0.369230769230769</v>
-      </c>
-      <c r="I4" s="28" t="inlineStr">
+        <v>0.36923076923077</v>
+      </c>
+      <c r="I4" s="29" t="inlineStr">
         <f aca="false">H4+I3</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
-      <c r="G5" s="30"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
-      <c r="A6" s="37" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
+      <c r="A6" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="22" t="n">
+      <c r="C6" s="23" t="n">
         <f aca="false">SUM(C2:C4)</f>
         <v>105</v>
       </c>
-      <c r="D6" s="22" t="n">
+      <c r="D6" s="23" t="n">
         <f aca="false">SUM(D2:D4)</f>
         <v>97.5</v>
       </c>
-      <c r="G6" s="30" t="n">
+      <c r="G6" s="25" t="inlineStr">
         <f aca="false">SUM(G2:G4)</f>
-        <v>72.65</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -7164,16 +7542,16 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G13" activeCellId="0" pane="topLeft" sqref="G13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G38" activeCellId="0" pane="topLeft" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="22" width="15.6274509803922"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="2.60392156862745"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="22" width="15.6274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="22" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="23" width="15.7098039215686"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="2.6156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="23" width="15.7098039215686"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="23" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1">
@@ -7218,199 +7596,199 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="26" t="n">
+      <c r="A2" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="n">
+      <c r="B2" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hetl)</f>
         <v>6.5</v>
       </c>
-      <c r="C2" s="26" t="n">
+      <c r="C2" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hedm)</f>
         <v>7</v>
       </c>
-      <c r="D2" s="26" t="n">
+      <c r="D2" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hepqm)</f>
         <v>5.5</v>
       </c>
-      <c r="E2" s="26" t="n">
+      <c r="E2" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hepm)</f>
         <v>11.5</v>
       </c>
-      <c r="F2" s="26" t="n">
+      <c r="F2" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hesm)</f>
         <v>5.5</v>
       </c>
-      <c r="G2" s="26" t="n">
+      <c r="G2" s="27" t="n">
         <f aca="false">SUM(B2:F2)</f>
         <v>36</v>
       </c>
-      <c r="I2" s="26" t="n">
+      <c r="I2" s="27" t="n">
         <v>2.35</v>
       </c>
-      <c r="J2" s="26" t="n">
+      <c r="J2" s="27" t="n">
         <v>2.1</v>
       </c>
-      <c r="K2" s="26" t="n">
+      <c r="K2" s="27" t="n">
         <v>3.93</v>
       </c>
-      <c r="L2" s="26" t="n">
+      <c r="L2" s="27" t="n">
         <v>7.42</v>
       </c>
-      <c r="M2" s="26" t="n">
+      <c r="M2" s="27" t="n">
         <v>5.27</v>
       </c>
-      <c r="N2" s="26" t="n">
+      <c r="N2" s="27" t="n">
         <f aca="false">SUM(I2:M2)</f>
         <v>21.07</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="26" t="n">
+      <c r="A3" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="n">
+      <c r="B3" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hetl)</f>
         <v>5</v>
       </c>
-      <c r="C3" s="26" t="n">
+      <c r="C3" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hedm)</f>
         <v>10</v>
       </c>
-      <c r="D3" s="26" t="n">
+      <c r="D3" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hepqm)</f>
         <v>7</v>
       </c>
-      <c r="E3" s="26" t="n">
+      <c r="E3" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hepm)</f>
         <v>6.5</v>
       </c>
-      <c r="F3" s="26" t="n">
+      <c r="F3" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hesm)</f>
         <v>5</v>
       </c>
-      <c r="G3" s="26" t="n">
+      <c r="G3" s="27" t="n">
         <f aca="false">SUM(B3:F3)</f>
         <v>33.5</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="I3" s="27" t="n">
         <v>7.33</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="J3" s="27" t="n">
         <v>7.28</v>
       </c>
-      <c r="K3" s="26" t="n">
+      <c r="K3" s="27" t="n">
         <v>5.33</v>
       </c>
-      <c r="L3" s="26" t="n">
+      <c r="L3" s="27" t="n">
         <v>4.42</v>
       </c>
-      <c r="M3" s="26" t="n">
+      <c r="M3" s="27" t="n">
         <v>4.67</v>
       </c>
-      <c r="N3" s="26" t="n">
+      <c r="N3" s="27" t="n">
         <f aca="false">SUM(I3:M3)</f>
         <v>29.03</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="26" t="n">
+      <c r="A4" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="n">
+      <c r="B4" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hetl)</f>
         <v>8.5</v>
       </c>
-      <c r="C4" s="26" t="n">
+      <c r="C4" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hedm)</f>
         <v>9.5</v>
       </c>
-      <c r="D4" s="26" t="n">
+      <c r="D4" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hepqm)</f>
         <v>3</v>
       </c>
-      <c r="E4" s="26" t="n">
+      <c r="E4" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hepm)</f>
         <v>3</v>
       </c>
-      <c r="F4" s="26" t="n">
+      <c r="F4" s="27" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hesm)</f>
         <v>4</v>
       </c>
-      <c r="G4" s="26" t="n">
+      <c r="G4" s="27" t="n">
         <f aca="false">SUM(B4:F4)</f>
         <v>28</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="I4" s="27" t="n">
         <v>5.43</v>
       </c>
-      <c r="J4" s="26" t="n">
+      <c r="J4" s="27" t="n">
         <v>8.72</v>
       </c>
-      <c r="K4" s="26" t="n">
+      <c r="K4" s="27" t="n">
         <v>10.12</v>
       </c>
-      <c r="L4" s="26" t="n">
+      <c r="L4" s="27" t="n">
         <v>10.5</v>
       </c>
-      <c r="M4" s="26" t="n">
+      <c r="M4" s="27" t="n">
         <v>5.87</v>
       </c>
-      <c r="N4" s="26" t="n">
+      <c r="N4" s="27" t="n">
         <f aca="false">SUM(I4:M4)</f>
         <v>40.64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5" s="22"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
-      <c r="A6" s="37" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5" s="23"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
+      <c r="A6" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="22" t="n">
+      <c r="B6" s="23" t="n">
         <f aca="false">SUM(B2:B4)</f>
         <v>20</v>
       </c>
-      <c r="C6" s="22" t="n">
+      <c r="C6" s="23" t="n">
         <f aca="false">SUM(C2:C4)</f>
         <v>26.5</v>
       </c>
-      <c r="D6" s="22" t="n">
+      <c r="D6" s="23" t="n">
         <f aca="false">SUM(D2:D4)</f>
         <v>15.5</v>
       </c>
-      <c r="E6" s="22" t="n">
+      <c r="E6" s="23" t="n">
         <f aca="false">SUM(E2:E4)</f>
         <v>21</v>
       </c>
-      <c r="F6" s="22" t="n">
+      <c r="F6" s="23" t="n">
         <f aca="false">SUM(F2:F4)</f>
         <v>14.5</v>
       </c>
-      <c r="G6" s="22" t="n">
+      <c r="G6" s="23" t="n">
         <f aca="false">SUM(G2:G4)</f>
         <v>97.5</v>
       </c>
-      <c r="I6" s="22" t="n">
+      <c r="I6" s="23" t="n">
         <f aca="false">SUM(I2:I4)</f>
         <v>15.11</v>
       </c>
-      <c r="J6" s="22" t="n">
+      <c r="J6" s="23" t="n">
         <f aca="false">SUM(J2:J4)</f>
         <v>18.1</v>
       </c>
-      <c r="K6" s="22" t="n">
+      <c r="K6" s="23" t="n">
         <f aca="false">SUM(K2:K4)</f>
         <v>19.38</v>
       </c>
-      <c r="L6" s="22" t="n">
+      <c r="L6" s="23" t="n">
         <f aca="false">SUM(L2:L4)</f>
         <v>22.34</v>
       </c>
-      <c r="M6" s="22" t="n">
+      <c r="M6" s="23" t="n">
         <f aca="false">SUM(M2:M4)</f>
         <v>15.81</v>
       </c>
-      <c r="N6" s="22" t="n">
+      <c r="N6" s="23" t="n">
         <f aca="false">SUM(N2:N4)</f>
         <v>90.74</v>
       </c>

</xml_diff>

<commit_message>
Launch, strategy, plan del ciclo #2.
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="439" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="439" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="tareas" sheetId="1" state="visible" r:id="rId2"/>
@@ -569,7 +569,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -616,9 +616,6 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
@@ -646,6 +643,8 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
@@ -730,7 +729,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -830,16 +829,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.217522658610272</c:v>
+                  <c:v>0.220183486238532</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.419939577039275</c:v>
+                  <c:v>0.425076452599388</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.589123867069486</c:v>
+                  <c:v>0.596330275229358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.845921450151057</c:v>
+                  <c:v>0.844036697247706</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -940,48 +939,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.138972809667674</c:v>
+                  <c:v>0.140672782874618</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.220543806646526</c:v>
+                  <c:v>0.223241590214067</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.438066465256798</c:v>
+                  <c:v>0.443425076452599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58807470"/>
-        <c:axId val="9345397"/>
+        <c:axId val="52477798"/>
+        <c:axId val="18198914"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58807470"/>
+        <c:axId val="52477798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -989,7 +988,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9345397"/>
+        <c:crossAx val="18198914"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1003,7 +1002,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9345397"/>
+        <c:axId val="18198914"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1019,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58807470"/>
+        <c:crossAx val="52477798"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1052,7 +1051,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1258,7 +1257,7 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.5</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>25.5</c:v>
@@ -1389,11 +1388,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="14217580"/>
-        <c:axId val="20667980"/>
+        <c:axId val="32871529"/>
+        <c:axId val="46502873"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14217580"/>
+        <c:axId val="32871529"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="20667980"/>
+        <c:crossAx val="46502873"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1415,7 +1414,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20667980"/>
+        <c:axId val="46502873"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,7 +1431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="14217580"/>
+        <c:crossAx val="32871529"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1464,7 +1463,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1605,21 +1604,21 @@
                   <c:v>0.235897435897436</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.374358974358974</c:v>
+                  <c:v>0.374358974358975</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.743589743589743</c:v>
+                  <c:v>0.743589743589745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90399656"/>
-        <c:axId val="67441229"/>
+        <c:axId val="67798587"/>
+        <c:axId val="40039017"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90399656"/>
+        <c:axId val="67798587"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,7 +1626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67441229"/>
+        <c:crossAx val="40039017"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1641,7 +1640,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67441229"/>
+        <c:axId val="40039017"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1657,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90399656"/>
+        <c:crossAx val="67798587"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1690,7 +1689,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1824,21 +1823,21 @@
                   <c:v>0.235897435897436</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.138461538461538</c:v>
+                  <c:v>0.138461538461539</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.369230769230769</c:v>
+                  <c:v>0.36923076923077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="12858955"/>
-        <c:axId val="97040498"/>
+        <c:axId val="78292454"/>
+        <c:axId val="57181481"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="12858955"/>
+        <c:axId val="78292454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1846,7 +1845,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97040498"/>
+        <c:crossAx val="57181481"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1860,7 +1859,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97040498"/>
+        <c:axId val="57181481"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1877,7 +1876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="12858955"/>
+        <c:crossAx val="78292454"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1909,7 +1908,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2047,11 +2046,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="9831491"/>
-        <c:axId val="38958556"/>
+        <c:axId val="38884848"/>
+        <c:axId val="50668725"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="9831491"/>
+        <c:axId val="38884848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2059,7 +2058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38958556"/>
+        <c:crossAx val="50668725"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -2073,7 +2072,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38958556"/>
+        <c:axId val="50668725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9831491"/>
+        <c:crossAx val="38884848"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2122,7 +2121,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2260,11 +2259,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="55636552"/>
-        <c:axId val="96718647"/>
+        <c:axId val="24361275"/>
+        <c:axId val="44977840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55636552"/>
+        <c:axId val="24361275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2271,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96718647"/>
+        <c:crossAx val="44977840"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -2286,7 +2285,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96718647"/>
+        <c:axId val="44977840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2303,7 +2302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55636552"/>
+        <c:crossAx val="24361275"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2335,7 +2334,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2439,11 +2438,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="54964556"/>
-        <c:axId val="82855311"/>
+        <c:axId val="70230140"/>
+        <c:axId val="37968845"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54964556"/>
+        <c:axId val="70230140"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2450,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82855311"/>
+        <c:crossAx val="37968845"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -2465,7 +2464,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82855311"/>
+        <c:axId val="37968845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2482,7 +2481,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54964556"/>
+        <c:crossAx val="70230140"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2514,7 +2513,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2652,11 +2651,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="42665869"/>
-        <c:axId val="53620963"/>
+        <c:axId val="60508736"/>
+        <c:axId val="46114025"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42665869"/>
+        <c:axId val="60508736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2664,7 +2663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53620963"/>
+        <c:crossAx val="46114025"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -2678,7 +2677,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53620963"/>
+        <c:axId val="46114025"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,7 +2694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42665869"/>
+        <c:crossAx val="60508736"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2727,7 +2726,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2865,11 +2864,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="50658730"/>
-        <c:axId val="64270945"/>
+        <c:axId val="30862117"/>
+        <c:axId val="55355452"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50658730"/>
+        <c:axId val="30862117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2877,7 +2876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64270945"/>
+        <c:crossAx val="55355452"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -2891,7 +2890,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64270945"/>
+        <c:axId val="55355452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2908,7 +2907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50658730"/>
+        <c:crossAx val="30862117"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2940,7 +2939,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3078,11 +3077,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="34601567"/>
-        <c:axId val="42590453"/>
+        <c:axId val="72280498"/>
+        <c:axId val="77427935"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34601567"/>
+        <c:axId val="72280498"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3090,7 +3089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42590453"/>
+        <c:crossAx val="77427935"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -3104,7 +3103,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42590453"/>
+        <c:axId val="77427935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3121,7 +3120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="34601567"/>
+        <c:crossAx val="72280498"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -3153,7 +3152,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3438,11 +3437,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="25199999"/>
-        <c:axId val="77744924"/>
+        <c:axId val="9654239"/>
+        <c:axId val="66301838"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="25199999"/>
+        <c:axId val="9654239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3450,8 +3449,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77744924"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="66301838"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -3464,7 +3463,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77744924"/>
+        <c:axId val="66301838"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3481,8 +3480,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="25199999"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9654239"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -3518,15 +3517,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:colOff>430200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:colOff>409320</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3534,8 +3533,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="249120" y="2667960"/>
-        <a:ext cx="10788120" cy="3024360"/>
+        <a:off x="430200" y="3189960"/>
+        <a:ext cx="10895400" cy="2594520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3548,15 +3547,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:colOff>408960</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:colOff>345600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3564,8 +3563,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="323280" y="6363720"/>
-        <a:ext cx="10745640" cy="3457440"/>
+        <a:off x="408960" y="7429680"/>
+        <a:ext cx="10852920" cy="2998440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3583,15 +3582,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:colOff>282960</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>479160</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:colOff>532440</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3599,8 +3598,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="228960" y="1508400"/>
-        <a:ext cx="8043480" cy="2613960"/>
+        <a:off x="282960" y="709560"/>
+        <a:ext cx="8120160" cy="2248200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3613,15 +3612,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>287640</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:colOff>341640</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>469440</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:colOff>522720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3629,8 +3628,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="287640" y="4222800"/>
-        <a:ext cx="7975080" cy="2613240"/>
+        <a:off x="341640" y="3047040"/>
+        <a:ext cx="8051760" cy="2262240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3648,15 +3647,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>280440</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:colOff>334440</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>530640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>841320</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:colOff>894600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3664,8 +3663,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="280440" y="1635120"/>
-        <a:ext cx="5789160" cy="3023280"/>
+        <a:off x="334440" y="530640"/>
+        <a:ext cx="5842440" cy="2609280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3678,15 +3677,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>385920</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:colOff>439920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>946800</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:colOff>1000080</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3694,8 +3693,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="385920" y="4874040"/>
-        <a:ext cx="5789160" cy="3023280"/>
+        <a:off x="439920" y="3319920"/>
+        <a:ext cx="5842440" cy="2624760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3708,15 +3707,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:colOff>434880</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>938520</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:colOff>991800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3724,8 +3723,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="380880" y="8197560"/>
-        <a:ext cx="5785920" cy="3022200"/>
+        <a:off x="434880" y="6197040"/>
+        <a:ext cx="5839200" cy="2623320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3738,15 +3737,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>415800</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:colOff>469800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>973440</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:colOff>1026720</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3754,8 +3753,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="415800" y="11587320"/>
-        <a:ext cx="5785920" cy="3022200"/>
+        <a:off x="469800" y="9140760"/>
+        <a:ext cx="5839200" cy="2623320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3768,15 +3767,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>458640</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:colOff>512640</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1016280</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:colOff>1069560</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>55800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3784,8 +3783,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="458640" y="14978520"/>
-        <a:ext cx="5785920" cy="3022200"/>
+        <a:off x="512640" y="12085200"/>
+        <a:ext cx="5839200" cy="2611440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3797,16 +3796,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>182520</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>51840</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>496080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>272520</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:colOff>325800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3814,8 +3813,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7616880" y="1600560"/>
-        <a:ext cx="5788440" cy="3009600"/>
+        <a:off x="7749000" y="496080"/>
+        <a:ext cx="5846040" cy="2595600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3828,15 +3827,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>61920</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:colOff>115920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>306720</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3844,8 +3843,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7679880" y="5002920"/>
-        <a:ext cx="5759640" cy="3236760"/>
+        <a:off x="7813080" y="3436560"/>
+        <a:ext cx="5816160" cy="2801880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3865,21 +3864,22 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E30" activeCellId="0" pane="topLeft" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.58039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="40.6627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.6156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.7254901960784"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="21.7254901960784"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="1023" min="12" style="4" width="12.0470588235294"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.61960784313725"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="41.0705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.9058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.9058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.65098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.9411764705882"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="21.9411764705882"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="1023" min="12" style="4" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.5921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -3889,7 +3889,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="8" t="n">
         <f aca="false">SUM(E3:E45)</f>
-        <v>165.5</v>
+        <v>163.5</v>
       </c>
       <c r="F1" s="9" t="inlineStr">
         <f aca="false">SUM(F3:F45)</f>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="F3" s="9" t="n">
         <f aca="false">E3/E1</f>
-        <v>0.0453172205438066</v>
+        <v>0.0458715596330275</v>
       </c>
       <c r="G3" s="14" t="n">
         <v>1</v>
@@ -3973,7 +3973,7 @@
           <t/>
         </is>
       </c>
-      <c r="K3" s="16" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <f aca="false">'tareas-ciclo1'!Q4</f>
         <is>
           <t/>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="F4" s="9" t="n">
         <f aca="false">E4/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G4" s="14" t="n">
         <v>1</v>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="F5" s="9" t="n">
         <f aca="false">E5/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G5" s="14" t="n">
         <v>1</v>
@@ -4074,7 +4074,7 @@
       </c>
       <c r="F6" s="9" t="n">
         <f aca="false">E6/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G6" s="14" t="n">
         <v>1</v>
@@ -4094,28 +4094,28 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7" s="19">
       <c r="A7" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F7" s="9" t="n">
         <f aca="false">E7/E1</f>
-        <v>0.00302114803625378</v>
-      </c>
-      <c r="G7" s="19" t="n">
+        <v>0.00305810397553517</v>
+      </c>
+      <c r="G7" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="18" t="n">
+      <c r="I7" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O8</f>
         <v>0.25</v>
       </c>
@@ -4130,32 +4130,32 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="19">
       <c r="A8" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="18" t="n">
+      <c r="E8" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F8" s="9" t="n">
         <f aca="false">E8/E1</f>
-        <v>0.00302114803625378</v>
-      </c>
-      <c r="G8" s="18" t="n">
+        <v>0.00305810397553517</v>
+      </c>
+      <c r="G8" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="18" t="n">
+      <c r="I8" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O9</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="J8" s="21" t="inlineStr">
+      <c r="J8" s="20" t="inlineStr">
         <f aca="false">F8</f>
         <is>
           <t/>
@@ -4166,34 +4166,34 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="19">
       <c r="A9" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F9" s="9" t="n">
         <f aca="false">E9/E1</f>
-        <v>0.00302114803625378</v>
-      </c>
-      <c r="G9" s="18" t="n">
+        <v>0.00305810397553517</v>
+      </c>
+      <c r="G9" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="18" t="n">
+      <c r="I9" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O10</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="J9" s="21" t="inlineStr">
+      <c r="J9" s="20" t="inlineStr">
         <f aca="false">F9</f>
         <is>
           <t/>
@@ -4204,34 +4204,34 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="19">
       <c r="A10" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="18" t="n">
+      <c r="E10" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">E10/E1</f>
-        <v>0.0120845921450151</v>
-      </c>
-      <c r="G10" s="18" t="n">
+        <v>0.0122324159021407</v>
+      </c>
+      <c r="G10" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="18" t="n">
+      <c r="I10" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O11</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J10" s="21" t="inlineStr">
+      <c r="J10" s="20" t="inlineStr">
         <f aca="false">F10</f>
         <is>
           <t/>
@@ -4242,68 +4242,68 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="19">
       <c r="A11" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="18" t="n">
+      <c r="E11" s="17" t="n">
         <v>3</v>
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">E11/E1</f>
-        <v>0.0181268882175227</v>
-      </c>
-      <c r="G11" s="18" t="n">
+        <v>0.018348623853211</v>
+      </c>
+      <c r="G11" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="18" t="n">
+      <c r="I11" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O12</f>
         <v>3.9</v>
       </c>
-      <c r="J11" s="21" t="inlineStr">
+      <c r="J11" s="20" t="inlineStr">
         <f aca="false">F11</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K11" s="18" t="n">
+      <c r="K11" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!Q12</f>
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="19">
       <c r="A12" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="17" t="n">
         <v>10</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">E12/E1</f>
-        <v>0.0604229607250755</v>
-      </c>
-      <c r="G12" s="18" t="n">
+        <v>0.0611620795107034</v>
+      </c>
+      <c r="G12" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="18" t="n">
+      <c r="I12" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O13</f>
         <v>0</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="18" t="n">
+      <c r="J12" s="20"/>
+      <c r="K12" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!Q13</f>
         <v>1</v>
       </c>
@@ -4312,10 +4312,10 @@
       <c r="A13" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="1" t="n">
@@ -4323,7 +4323,7 @@
       </c>
       <c r="F13" s="3" t="n">
         <f aca="false">E13/E1</f>
-        <v>0.0906344410876133</v>
+        <v>0.091743119266055</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>2</v>
@@ -4337,242 +4337,242 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="19">
       <c r="A14" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18" t="n">
+      <c r="D14" s="16"/>
+      <c r="E14" s="17" t="n">
         <v>10</v>
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">E14/E1</f>
-        <v>0.0604229607250755</v>
-      </c>
-      <c r="G14" s="18" t="n">
+        <v>0.0611620795107034</v>
+      </c>
+      <c r="G14" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="18" t="n">
+      <c r="I14" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O15</f>
         <v>8</v>
       </c>
-      <c r="J14" s="21" t="inlineStr">
+      <c r="J14" s="20" t="inlineStr">
         <f aca="false">F14</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K14" s="18" t="n">
+      <c r="K14" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!Q15</f>
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="19">
       <c r="A15" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="18" t="n">
+      <c r="E15" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">E15/E1</f>
-        <v>0.0120845921450151</v>
-      </c>
-      <c r="G15" s="18" t="n">
+        <v>0.0122324159021407</v>
+      </c>
+      <c r="G15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="19" t="n">
+      <c r="I15" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!O16</f>
         <v>15.4166666666667</v>
       </c>
-      <c r="J15" s="22" t="inlineStr">
+      <c r="J15" s="21" t="inlineStr">
         <f aca="false">SUM(F15:F17)</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K15" s="19" t="n">
+      <c r="K15" s="18" t="n">
         <f aca="false">'tareas-ciclo1'!Q16</f>
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="19">
       <c r="A16" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="18" t="n">
+      <c r="E16" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">E16/E1</f>
-        <v>0.0120845921450151</v>
-      </c>
-      <c r="G16" s="18" t="n">
+        <v>0.0122324159021407</v>
+      </c>
+      <c r="G16" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="17" s="20">
+      <c r="I16" s="18"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="17" s="19">
       <c r="A17" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="18" t="n">
+      <c r="E17" s="17" t="n">
         <v>4</v>
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">E17/E1</f>
-        <v>0.0241691842900302</v>
-      </c>
-      <c r="G17" s="18" t="n">
+        <v>0.0244648318042813</v>
+      </c>
+      <c r="G17" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18" s="20">
+      <c r="I17" s="18"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18" s="19">
       <c r="A18" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E18" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">E18/E1</f>
-        <v>0.00302114803625378</v>
-      </c>
-      <c r="G18" s="18" t="n">
+        <v>0.00305810397553517</v>
+      </c>
+      <c r="G18" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I18" s="18" t="n">
+      <c r="I18" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O19</f>
         <v>0.383333333333333</v>
       </c>
-      <c r="J18" s="21" t="inlineStr">
+      <c r="J18" s="20" t="inlineStr">
         <f aca="false">F18</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K18" s="18" t="n">
+      <c r="K18" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!Q19</f>
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="19">
       <c r="A19" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="18" t="n">
+      <c r="E19" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">E19/E1</f>
-        <v>0.0120845921450151</v>
-      </c>
-      <c r="G19" s="18" t="n">
+        <v>0.0122324159021407</v>
+      </c>
+      <c r="G19" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="I19" s="18" t="n">
+      <c r="I19" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O20</f>
         <v>1</v>
       </c>
-      <c r="J19" s="21" t="inlineStr">
+      <c r="J19" s="20" t="inlineStr">
         <f aca="false">F19</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K19" s="18" t="n">
+      <c r="K19" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!Q20</f>
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="19">
       <c r="A20" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18" t="n">
+      <c r="D20" s="16"/>
+      <c r="E20" s="17" t="n">
         <v>10</v>
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">E20/E1</f>
-        <v>0.0604229607250755</v>
-      </c>
-      <c r="G20" s="18" t="n">
+        <v>0.0611620795107034</v>
+      </c>
+      <c r="G20" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="I20" s="18" t="n">
+      <c r="I20" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!O21</f>
         <v>8.16666666666665</v>
       </c>
-      <c r="J20" s="21" t="inlineStr">
+      <c r="J20" s="20" t="inlineStr">
         <f aca="false">F20</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K20" s="18" t="n">
+      <c r="K20" s="17" t="n">
         <f aca="false">'tareas-ciclo1'!Q21</f>
         <v>3</v>
       </c>
@@ -4595,7 +4595,7 @@
       </c>
       <c r="F21" s="9" t="n">
         <f aca="false">E21/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G21" s="1" t="n">
         <v>3</v>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="F22" s="9" t="n">
         <f aca="false">E22/E1</f>
-        <v>0.0181268882175227</v>
+        <v>0.018348623853211</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>3</v>
@@ -4671,7 +4671,7 @@
       </c>
       <c r="F23" s="9" t="n">
         <f aca="false">E23/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G23" s="1" t="n">
         <v>3</v>
@@ -4709,7 +4709,7 @@
       </c>
       <c r="F24" s="9" t="n">
         <f aca="false">E24/E1</f>
-        <v>0.0241691842900302</v>
+        <v>0.0244648318042813</v>
       </c>
       <c r="G24" s="1" t="n">
         <v>3</v>
@@ -4733,7 +4733,7 @@
       <c r="A25" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -4747,7 +4747,7 @@
       </c>
       <c r="F25" s="9" t="n">
         <f aca="false">E25/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>3</v>
@@ -4771,7 +4771,7 @@
       <c r="A26" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>68</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="F26" s="9" t="n">
         <f aca="false">E26/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>4</v>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="F27" s="9" t="n">
         <f aca="false">E27/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>4</v>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="F28" s="9" t="n">
         <f aca="false">E28/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>4</v>
@@ -4850,11 +4850,11 @@
         <v>72</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" s="9" t="n">
         <f aca="false">E29/E1</f>
-        <v>0.0181268882175227</v>
+        <v>0.00611620795107034</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>4</v>
@@ -4875,7 +4875,7 @@
       </c>
       <c r="F30" s="9" t="n">
         <f aca="false">E30/E1</f>
-        <v>0.0604229607250755</v>
+        <v>0.0611620795107034</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>4</v>
@@ -4899,7 +4899,7 @@
       </c>
       <c r="F31" s="9" t="n">
         <f aca="false">E31/E1</f>
-        <v>0.00604229607250755</v>
+        <v>0.00611620795107034</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>4</v>
@@ -4923,7 +4923,7 @@
       </c>
       <c r="F32" s="9" t="n">
         <f aca="false">E32/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>4</v>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="F33" s="9" t="n">
         <f aca="false">E33/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>4</v>
@@ -4971,7 +4971,7 @@
       </c>
       <c r="F34" s="9" t="n">
         <f aca="false">E34/E1</f>
-        <v>0.0241691842900302</v>
+        <v>0.0244648318042813</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>4</v>
@@ -4984,10 +4984,10 @@
       <c r="B35" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="16" t="s">
         <v>85</v>
       </c>
       <c r="E35" s="1" t="n">
@@ -4995,7 +4995,7 @@
       </c>
       <c r="F35" s="3" t="n">
         <f aca="false">E35/E1</f>
-        <v>0.00302114803625378</v>
+        <v>0.00305810397553517</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>4</v>
@@ -5008,10 +5008,10 @@
       <c r="B36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="16" t="s">
         <v>88</v>
       </c>
       <c r="E36" s="1" t="n">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="F36" s="3" t="n">
         <f aca="false">E36/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>4</v>
@@ -5043,7 +5043,7 @@
       </c>
       <c r="F37" s="3" t="n">
         <f aca="false">E37/E1</f>
-        <v>0.0181268882175227</v>
+        <v>0.018348623853211</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>4</v>
@@ -5056,7 +5056,7 @@
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E38" s="1" t="n">
@@ -5064,7 +5064,7 @@
       </c>
       <c r="F38" s="3" t="n">
         <f aca="false">E38/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>5</v>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="F39" s="3" t="n">
         <f aca="false">E39/E1</f>
-        <v>0.00604229607250755</v>
+        <v>0.00611620795107034</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>5</v>
@@ -5112,7 +5112,7 @@
       </c>
       <c r="F40" s="3" t="n">
         <f aca="false">E40/E1</f>
-        <v>0.0302114803625378</v>
+        <v>0.0305810397553517</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>5</v>
@@ -5130,7 +5130,7 @@
       </c>
       <c r="F41" s="3" t="n">
         <f aca="false">E41/E1</f>
-        <v>0.0241691842900302</v>
+        <v>0.0244648318042813</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>5</v>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="F42" s="3" t="n">
         <f aca="false">E42/E1</f>
-        <v>0.0241691842900302</v>
+        <v>0.0244648318042813</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>5</v>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="F43" s="3" t="n">
         <f aca="false">E43/E1</f>
-        <v>0.0241691842900302</v>
+        <v>0.0244648318042813</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>5</v>
@@ -5184,7 +5184,7 @@
       </c>
       <c r="F44" s="3" t="n">
         <f aca="false">E44/E1</f>
-        <v>0.00302114803625378</v>
+        <v>0.00305810397553517</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>5</v>
@@ -5202,7 +5202,7 @@
       </c>
       <c r="F45" s="3" t="n">
         <f aca="false">E45/E1</f>
-        <v>0.0120845921450151</v>
+        <v>0.0122324159021407</v>
       </c>
       <c r="G45" s="1" t="n">
         <v>5</v>
@@ -5231,24 +5231,24 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I50" activeCellId="0" pane="topLeft" sqref="I50"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G15" activeCellId="0" pane="topLeft" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="17.0666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.7607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="18.4941176470588"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="25" width="21.4705882352941"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="23" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="12.8627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="17.2313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="19.9607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.678431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="24" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="22" width="12.8627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -5274,25 +5274,25 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="27" t="n">
+      <c r="A2" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="27" t="n">
         <v>41902</v>
       </c>
-      <c r="C2" s="27" t="n">
+      <c r="C2" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D2" s="27" t="n">
+      <c r="D2" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A2,_gTDHE)</f>
         <v>36</v>
       </c>
-      <c r="E2" s="29" t="n">
+      <c r="E2" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A2,_gPIDGE)</f>
-        <v>0.217522658610272</v>
-      </c>
-      <c r="F2" s="29" t="inlineStr">
+        <v>0.220183486238532</v>
+      </c>
+      <c r="F2" s="28" t="inlineStr">
         <f aca="false">E2</f>
         <is>
           <t/>
@@ -5302,11 +5302,11 @@
         <f aca="false">SUMIF(_gSR,A2,_gTDHT)</f>
         <v>17.65</v>
       </c>
-      <c r="H2" s="29" t="n">
+      <c r="H2" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A2,_gPIDGO)</f>
-        <v>0.138972809667674</v>
-      </c>
-      <c r="I2" s="29" t="inlineStr">
+        <v>0.140672782874618</v>
+      </c>
+      <c r="I2" s="28" t="inlineStr">
         <f aca="false">H2</f>
         <is>
           <t/>
@@ -5314,28 +5314,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="27" t="n">
+      <c r="A3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="inlineStr">
+      <c r="B3" s="27" t="inlineStr">
         <f aca="false">B2+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A3,_gTDHE)</f>
         <v>33.5</v>
       </c>
-      <c r="E3" s="29" t="n">
+      <c r="E3" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A3,_gPIDGE)</f>
-        <v>0.202416918429003</v>
-      </c>
-      <c r="F3" s="29" t="inlineStr">
+        <v>0.204892966360856</v>
+      </c>
+      <c r="F3" s="28" t="inlineStr">
         <f aca="false">E3+F2</f>
         <is>
           <t/>
@@ -5345,11 +5345,11 @@
         <f aca="false">SUMIF(_gSR,A3,_gTDHT)</f>
         <v>15.1166666666667</v>
       </c>
-      <c r="H3" s="29" t="n">
+      <c r="H3" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A3,_gPIDGO)</f>
-        <v>0.081570996978852</v>
-      </c>
-      <c r="I3" s="29" t="inlineStr">
+        <v>0.0825688073394496</v>
+      </c>
+      <c r="I3" s="28" t="inlineStr">
         <f aca="false">H3+I2</f>
         <is>
           <t/>
@@ -5357,28 +5357,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="27" t="n">
+      <c r="A4" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="inlineStr">
+      <c r="B4" s="27" t="inlineStr">
         <f aca="false">B3+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A4,_gTDHE)</f>
         <v>28</v>
       </c>
-      <c r="E4" s="29" t="n">
+      <c r="E4" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A4,_gPIDGE)</f>
-        <v>0.169184290030211</v>
-      </c>
-      <c r="F4" s="29" t="inlineStr">
+        <v>0.171253822629969</v>
+      </c>
+      <c r="F4" s="28" t="inlineStr">
         <f aca="false">E4+F3</f>
         <is>
           <t/>
@@ -5388,11 +5388,11 @@
         <f aca="false">SUMIF(_gSR,A4,_gTDHT)</f>
         <v>39.8833333333333</v>
       </c>
-      <c r="H4" s="29" t="n">
+      <c r="H4" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A4,_gPIDGO)</f>
-        <v>0.217522658610272</v>
-      </c>
-      <c r="I4" s="29" t="inlineStr">
+        <v>0.220183486238532</v>
+      </c>
+      <c r="I4" s="28" t="inlineStr">
         <f aca="false">H4+I3</f>
         <is>
           <t/>
@@ -5400,28 +5400,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
-      <c r="A5" s="27" t="n">
+      <c r="A5" s="26" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="inlineStr">
+      <c r="B5" s="27" t="inlineStr">
         <f aca="false">B4+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D5" s="27" t="n">
+      <c r="D5" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A5,_gTDHE)</f>
-        <v>42.5</v>
-      </c>
-      <c r="E5" s="29" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="E5" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A5,_gPIDGE)</f>
-        <v>0.256797583081571</v>
-      </c>
-      <c r="F5" s="29" t="inlineStr">
+        <v>0.247706422018349</v>
+      </c>
+      <c r="F5" s="28" t="inlineStr">
         <f aca="false">E5+F4</f>
         <is>
           <t/>
@@ -5431,11 +5431,11 @@
         <f aca="false">SUMIF(_gSR,A5,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="29" t="n">
+      <c r="H5" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A5,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="29" t="inlineStr">
+      <c r="I5" s="28" t="inlineStr">
         <f aca="false">H5+I4</f>
         <is>
           <t/>
@@ -5443,28 +5443,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="6">
-      <c r="A6" s="27" t="n">
+      <c r="A6" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="inlineStr">
+      <c r="B6" s="27" t="inlineStr">
         <f aca="false">B5+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C6" s="27" t="n">
+      <c r="C6" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D6" s="27" t="n">
+      <c r="D6" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A6,_gTDHE)</f>
         <v>25.5</v>
       </c>
-      <c r="E6" s="29" t="n">
+      <c r="E6" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A6,_gPIDGE)</f>
-        <v>0.154078549848943</v>
-      </c>
-      <c r="F6" s="29" t="inlineStr">
+        <v>0.155963302752294</v>
+      </c>
+      <c r="F6" s="28" t="inlineStr">
         <f aca="false">E6+F5</f>
         <is>
           <t/>
@@ -5474,11 +5474,11 @@
         <f aca="false">SUMIF(_gSR,A6,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="29" t="n">
+      <c r="H6" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A6,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="29" t="inlineStr">
+      <c r="I6" s="28" t="inlineStr">
         <f aca="false">H6+I5</f>
         <is>
           <t/>
@@ -5486,28 +5486,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="7">
-      <c r="A7" s="27" t="n">
+      <c r="A7" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="28" t="inlineStr">
+      <c r="B7" s="27" t="inlineStr">
         <f aca="false">B6+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C7" s="27" t="n">
+      <c r="C7" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D7" s="27" t="n">
+      <c r="D7" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A7,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="29" t="n">
+      <c r="E7" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A7,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="29" t="inlineStr">
+      <c r="F7" s="28" t="inlineStr">
         <f aca="false">E7+F6</f>
         <is>
           <t/>
@@ -5517,11 +5517,11 @@
         <f aca="false">SUMIF(_gSR,A7,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="29" t="n">
+      <c r="H7" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A7,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="29" t="inlineStr">
+      <c r="I7" s="28" t="inlineStr">
         <f aca="false">H7+I6</f>
         <is>
           <t/>
@@ -5529,28 +5529,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="8">
-      <c r="A8" s="27" t="n">
+      <c r="A8" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="28" t="inlineStr">
+      <c r="B8" s="27" t="inlineStr">
         <f aca="false">B7+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C8" s="27" t="n">
+      <c r="C8" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D8" s="27" t="n">
+      <c r="D8" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A8,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="29" t="n">
+      <c r="E8" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A8,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="29" t="inlineStr">
+      <c r="F8" s="28" t="inlineStr">
         <f aca="false">E8+F7</f>
         <is>
           <t/>
@@ -5560,11 +5560,11 @@
         <f aca="false">SUMIF(_gSR,A8,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="29" t="n">
+      <c r="H8" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A8,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="29" t="inlineStr">
+      <c r="I8" s="28" t="inlineStr">
         <f aca="false">H8+I7</f>
         <is>
           <t/>
@@ -5572,28 +5572,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="9">
-      <c r="A9" s="27" t="n">
+      <c r="A9" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="28" t="inlineStr">
+      <c r="B9" s="27" t="inlineStr">
         <f aca="false">B8+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C9" s="27" t="n">
+      <c r="C9" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D9" s="27" t="n">
+      <c r="D9" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A9,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="29" t="n">
+      <c r="E9" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A9,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="29" t="inlineStr">
+      <c r="F9" s="28" t="inlineStr">
         <f aca="false">E9+F8</f>
         <is>
           <t/>
@@ -5603,11 +5603,11 @@
         <f aca="false">SUMIF(_gSR,A9,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="29" t="n">
+      <c r="H9" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A9,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="29" t="inlineStr">
+      <c r="I9" s="28" t="inlineStr">
         <f aca="false">H9+I8</f>
         <is>
           <t/>
@@ -5615,28 +5615,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="10">
-      <c r="A10" s="27" t="n">
+      <c r="A10" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="inlineStr">
+      <c r="B10" s="27" t="inlineStr">
         <f aca="false">B9+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C10" s="27" t="n">
+      <c r="C10" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A10,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="29" t="n">
+      <c r="E10" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A10,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="29" t="inlineStr">
+      <c r="F10" s="28" t="inlineStr">
         <f aca="false">E10+F9</f>
         <is>
           <t/>
@@ -5646,11 +5646,11 @@
         <f aca="false">SUMIF(_gSR,A10,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="29" t="n">
+      <c r="H10" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A10,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="29" t="inlineStr">
+      <c r="I10" s="28" t="inlineStr">
         <f aca="false">H10+I9</f>
         <is>
           <t/>
@@ -5658,28 +5658,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="11">
-      <c r="A11" s="27" t="n">
+      <c r="A11" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="inlineStr">
+      <c r="B11" s="27" t="inlineStr">
         <f aca="false">B10+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C11" s="27" t="n">
+      <c r="C11" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D11" s="27" t="n">
+      <c r="D11" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A11,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="29" t="n">
+      <c r="E11" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A11,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="29" t="inlineStr">
+      <c r="F11" s="28" t="inlineStr">
         <f aca="false">E11+F10</f>
         <is>
           <t/>
@@ -5689,11 +5689,11 @@
         <f aca="false">SUMIF(_gSR,A11,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="29" t="n">
+      <c r="H11" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A11,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="29" t="inlineStr">
+      <c r="I11" s="28" t="inlineStr">
         <f aca="false">H11+I10</f>
         <is>
           <t/>
@@ -5701,28 +5701,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="12">
-      <c r="A12" s="27" t="n">
+      <c r="A12" s="26" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="28" t="inlineStr">
+      <c r="B12" s="27" t="inlineStr">
         <f aca="false">B11+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C12" s="27" t="n">
+      <c r="C12" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D12" s="27" t="n">
+      <c r="D12" s="26" t="n">
         <f aca="false">SUMIF(_gSE,A12,_gTDHE)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="29" t="n">
+      <c r="E12" s="28" t="n">
         <f aca="false">SUMIF(_gSE,A12,_gPIDGE)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="29" t="inlineStr">
+      <c r="F12" s="28" t="inlineStr">
         <f aca="false">E12+F11</f>
         <is>
           <t/>
@@ -5732,34 +5732,32 @@
         <f aca="false">SUMIF(_gSR,A12,_gTDHT)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="29" t="n">
+      <c r="H12" s="28" t="n">
         <f aca="false">SUMIF(_gSR,A12,_gPIDGO)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="29" t="inlineStr">
+      <c r="I12" s="28" t="inlineStr">
         <f aca="false">H12+I11</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="14">
       <c r="A14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="23" t="n">
+      <c r="C14" s="22" t="n">
         <f aca="false">SUM(C2:C12)</f>
         <v>385</v>
       </c>
-      <c r="D14" s="23" t="n">
+      <c r="D14" s="22" t="n">
         <f aca="false">SUM(D2:D12)</f>
-        <v>165.5</v>
-      </c>
-      <c r="G14" s="25" t="inlineStr">
+        <v>163.5</v>
+      </c>
+      <c r="G14" s="30" t="n">
         <f aca="false">SUM(G2:G12)</f>
-        <is>
-          <t/>
-        </is>
+        <v>72.65</v>
       </c>
     </row>
   </sheetData>
@@ -5786,19 +5784,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.6"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="40.6627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.73333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="20.3333333333333"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="2.73333333333333"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="4" width="2.73333333333333"/>
-    <col collapsed="false" hidden="false" max="23" min="19" style="4" width="20.3333333333333"/>
-    <col collapsed="false" hidden="false" max="1023" min="24" style="4" width="12.0470588235294"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.63529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="41.0705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.9058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.9058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="20.5411764705882"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="21.9058823529412"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="4" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="23" min="19" style="4" width="20.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1023" min="24" style="4" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.5921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -5834,7 +5833,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="30" t="n">
+      <c r="E2" s="31" t="n">
         <f aca="false">SUM(E4:E26)</f>
         <v>97.5</v>
       </c>
@@ -6222,34 +6221,34 @@
       </c>
       <c r="W7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="19">
       <c r="A8" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="18" t="n">
+      <c r="E8" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F8" s="9" t="n">
         <f aca="false">E8/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G8" s="19" t="n">
+      <c r="G8" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="18"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M8" s="18"/>
+      <c r="M8" s="17"/>
       <c r="O8" s="1" t="n">
         <f aca="false">SUM(S8:W8)</f>
         <v>0.25</v>
@@ -6260,47 +6259,47 @@
           <t/>
         </is>
       </c>
-      <c r="Q8" s="18" t="n">
+      <c r="Q8" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18" t="n">
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17" t="n">
         <f aca="false">15/60</f>
         <v>0.25</v>
       </c>
-      <c r="W8" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="20">
+      <c r="W8" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="19">
       <c r="A9" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F9" s="9" t="n">
         <f aca="false">E9/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G9" s="18" t="n">
+      <c r="G9" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M9" s="18"/>
+      <c r="M9" s="17"/>
       <c r="O9" s="1" t="n">
         <f aca="false">SUM(S9:W9)</f>
         <v>0.666666666666667</v>
@@ -6311,49 +6310,49 @@
           <t/>
         </is>
       </c>
-      <c r="Q9" s="18" t="n">
+      <c r="Q9" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18" t="n">
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="W9" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="20">
+      <c r="W9" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="19">
       <c r="A10" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="18" t="n">
+      <c r="E10" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">E10/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G10" s="18" t="n">
+      <c r="G10" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="M10" s="18"/>
+      <c r="M10" s="17"/>
       <c r="O10" s="1" t="n">
         <f aca="false">SUM(S10:W10)</f>
         <v>0.416666666666667</v>
@@ -6364,51 +6363,51 @@
           <t/>
         </is>
       </c>
-      <c r="Q10" s="18" t="n">
+      <c r="Q10" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18" t="n">
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17" t="n">
         <f aca="false">25/60</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="W10" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="20">
+      <c r="W10" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="19">
       <c r="A11" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="18" t="n">
+      <c r="E11" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">E11/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G11" s="18" t="n">
+      <c r="G11" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="18" t="n">
+      <c r="I11" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="18"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="18" t="n">
+      <c r="L11" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="18"/>
+      <c r="M11" s="17"/>
       <c r="O11" s="1" t="n">
         <f aca="false">SUM(S11:W11)</f>
         <v>1.16666666666667</v>
@@ -6419,52 +6418,52 @@
           <t/>
         </is>
       </c>
-      <c r="Q11" s="18" t="n">
+      <c r="Q11" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18" t="n">
+      <c r="R11" s="17"/>
+      <c r="S11" s="17" t="n">
         <f aca="false">35/60</f>
         <v>0.583333333333333</v>
       </c>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18" t="n">
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17" t="n">
         <f aca="false">35/60</f>
         <v>0.583333333333333</v>
       </c>
-      <c r="W11" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="20">
+      <c r="W11" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="19">
       <c r="A12" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="17" t="n">
         <v>3</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">E12/E2</f>
         <v>0.0307692307692308</v>
       </c>
-      <c r="G12" s="18" t="n">
+      <c r="G12" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18" t="n">
+      <c r="I12" s="17"/>
+      <c r="J12" s="17" t="n">
         <v>1.5</v>
       </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18" t="n">
+      <c r="K12" s="17"/>
+      <c r="L12" s="17" t="n">
         <v>1.5</v>
       </c>
-      <c r="M12" s="18"/>
+      <c r="M12" s="17"/>
       <c r="O12" s="1" t="n">
         <f aca="false">SUM(S12:W12)</f>
         <v>3.9</v>
@@ -6475,71 +6474,71 @@
           <t/>
         </is>
       </c>
-      <c r="Q12" s="18" t="n">
+      <c r="Q12" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18" t="n">
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17" t="n">
         <f aca="false">(45+72)/60</f>
         <v>1.95</v>
       </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18" t="n">
+      <c r="U12" s="17"/>
+      <c r="V12" s="17" t="n">
         <f aca="false">(45+72)/60</f>
         <v>1.95</v>
       </c>
-      <c r="W12" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13" s="20">
+      <c r="W12" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13" s="19">
       <c r="A13" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="18" t="n">
+      <c r="E13" s="17" t="n">
         <v>10</v>
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">E13/E2</f>
         <v>0.102564102564103</v>
       </c>
-      <c r="G13" s="18" t="n">
+      <c r="G13" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="18" t="n">
+      <c r="I13" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="J13" s="18" t="n">
+      <c r="J13" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="K13" s="18" t="n">
+      <c r="K13" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="L13" s="18" t="n">
+      <c r="L13" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="M13" s="18" t="n">
+      <c r="M13" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="O13" s="31" t="n">
+      <c r="O13" s="32" t="n">
         <f aca="false">SUM(S13:W13)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32" t="n">
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14">
       <c r="A14" s="14" t="n">
@@ -6548,7 +6547,7 @@
       <c r="B14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="1" t="n">
@@ -6576,12 +6575,12 @@
       <c r="M14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="O14" s="31" t="n">
+      <c r="O14" s="32" t="n">
         <f aca="false">SUM(S14:W14)</f>
         <v>2.83333333333333</v>
       </c>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31" t="n">
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32" t="n">
         <v>2</v>
       </c>
       <c r="R14" s="1"/>
@@ -6597,403 +6596,403 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15" s="19">
       <c r="A15" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18" t="n">
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">E15/E2</f>
         <v>0.102564102564103</v>
       </c>
-      <c r="G15" s="18" t="n">
+      <c r="G15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="18" t="n">
+      <c r="I15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="J15" s="18" t="n">
+      <c r="J15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="K15" s="18" t="n">
+      <c r="K15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="L15" s="18" t="n">
+      <c r="L15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="M15" s="18" t="n">
+      <c r="M15" s="17" t="n">
         <v>2</v>
       </c>
       <c r="O15" s="1" t="n">
         <f aca="false">SUM(S15:W15)</f>
         <v>8</v>
       </c>
-      <c r="P15" s="21" t="inlineStr">
+      <c r="P15" s="20" t="inlineStr">
         <f aca="false">F15</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q15" s="18" t="n">
+      <c r="Q15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18" t="n">
+      <c r="R15" s="17"/>
+      <c r="S15" s="17" t="n">
         <f aca="false">120/60</f>
         <v>2</v>
       </c>
-      <c r="T15" s="18" t="n">
+      <c r="T15" s="17" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
-      <c r="U15" s="18" t="n">
+      <c r="U15" s="17" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
-      <c r="V15" s="18" t="n">
+      <c r="V15" s="17" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
-      <c r="W15" s="18" t="n">
+      <c r="W15" s="17" t="n">
         <f aca="false">90/60</f>
         <v>1.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="19">
       <c r="A16" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="18" t="n">
+      <c r="E16" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">E16/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G16" s="18" t="n">
+      <c r="G16" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18" t="n">
+      <c r="I16" s="17"/>
+      <c r="J16" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18" t="n">
+      <c r="K16" s="17"/>
+      <c r="L16" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="M16" s="18"/>
+      <c r="M16" s="17"/>
       <c r="O16" s="14" t="n">
         <f aca="false">SUM(S16:W16)</f>
         <v>15.4166666666667</v>
       </c>
-      <c r="P16" s="22" t="inlineStr">
+      <c r="P16" s="21" t="inlineStr">
         <f aca="false">SUM(F16:F18)</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q16" s="19" t="n">
+      <c r="Q16" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="R16" s="18"/>
-      <c r="S16" s="19" t="n">
+      <c r="R16" s="17"/>
+      <c r="S16" s="18" t="n">
         <f aca="false">(40+75+90)/60</f>
         <v>3.41666666666667</v>
       </c>
-      <c r="T16" s="19" t="n">
+      <c r="T16" s="18" t="n">
         <f aca="false">(75+45+140)/60</f>
         <v>4.33333333333333</v>
       </c>
-      <c r="U16" s="19" t="n">
+      <c r="U16" s="18" t="n">
         <f aca="false">(120+50)/60</f>
         <v>2.83333333333333</v>
       </c>
-      <c r="V16" s="19" t="n">
+      <c r="V16" s="18" t="n">
         <f aca="false">75/60</f>
         <v>1.25</v>
       </c>
-      <c r="W16" s="19" t="n">
+      <c r="W16" s="18" t="n">
         <f aca="false">(140+75)/60</f>
         <v>3.58333333333333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="17" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="17" s="19">
       <c r="A17" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="18" t="n">
+      <c r="E17" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">E17/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G17" s="18" t="n">
+      <c r="G17" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18" t="n">
+      <c r="I17" s="17"/>
+      <c r="J17" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="18" s="20">
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="18" s="19">
       <c r="A18" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E18" s="17" t="n">
         <v>4</v>
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">E18/E2</f>
         <v>0.041025641025641</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G18" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18" t="n">
+      <c r="I18" s="17"/>
+      <c r="J18" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="K18" s="18" t="n">
+      <c r="K18" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
       <c r="O18" s="14"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="20">
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="19">
       <c r="A19" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="18" t="n">
+      <c r="E19" s="17" t="n">
         <v>0.5</v>
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">E19/E2</f>
         <v>0.00512820512820513</v>
       </c>
-      <c r="G19" s="18" t="n">
+      <c r="G19" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="L19" s="18" t="n">
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="L19" s="17" t="n">
         <v>0.5</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="M19" s="17"/>
       <c r="O19" s="1" t="n">
         <f aca="false">SUM(S19:W19)</f>
         <v>0.383333333333333</v>
       </c>
-      <c r="P19" s="21" t="inlineStr">
+      <c r="P19" s="20" t="inlineStr">
         <f aca="false">F19</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q19" s="18" t="n">
+      <c r="Q19" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18" t="n">
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17" t="n">
         <f aca="false">23/60</f>
         <v>0.383333333333333</v>
       </c>
-      <c r="W19" s="18"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="20">
+      <c r="W19" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="19">
       <c r="A20" s="14" t="n">
         <v>17</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="18" t="n">
+      <c r="E20" s="17" t="n">
         <v>2</v>
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">E20/E2</f>
         <v>0.0205128205128205</v>
       </c>
-      <c r="G20" s="18" t="n">
+      <c r="G20" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="I20" s="18" t="n">
+      <c r="I20" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18" t="n">
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="1" t="n">
         <f aca="false">SUM(S20:W20)</f>
         <v>1</v>
       </c>
-      <c r="P20" s="21" t="inlineStr">
+      <c r="P20" s="20" t="inlineStr">
         <f aca="false">F20</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q20" s="18" t="n">
+      <c r="Q20" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18" t="n">
+      <c r="R20" s="17"/>
+      <c r="S20" s="17" t="n">
         <f aca="false">30/60</f>
         <v>0.5</v>
       </c>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18" t="n">
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17" t="n">
         <f aca="false">30/60</f>
         <v>0.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="21" s="20">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="21" s="19">
       <c r="A21" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18" t="n">
+      <c r="D21" s="16"/>
+      <c r="E21" s="17" t="n">
         <v>10</v>
       </c>
       <c r="F21" s="9" t="n">
         <f aca="false">E21/E2</f>
         <v>0.102564102564103</v>
       </c>
-      <c r="G21" s="18" t="n">
+      <c r="G21" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="I21" s="18" t="n">
+      <c r="I21" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="J21" s="18" t="n">
+      <c r="J21" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="K21" s="18" t="n">
+      <c r="K21" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="L21" s="18" t="n">
+      <c r="L21" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="M21" s="18" t="n">
+      <c r="M21" s="17" t="n">
         <v>2</v>
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">SUM(S21:W21)</f>
         <v>8.16666666666665</v>
       </c>
-      <c r="P21" s="21" t="inlineStr">
+      <c r="P21" s="20" t="inlineStr">
         <f aca="false">F21</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="Q21" s="18" t="n">
+      <c r="Q21" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18" t="n">
+      <c r="R21" s="17"/>
+      <c r="S21" s="17" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="T21" s="18" t="n">
+      <c r="T21" s="17" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="U21" s="18" t="n">
+      <c r="U21" s="17" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="V21" s="18" t="n">
+      <c r="V21" s="17" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="W21" s="18" t="n">
+      <c r="W21" s="17" t="n">
         <f aca="false">98/60</f>
         <v>1.63333333333333</v>
       </c>
@@ -7028,7 +7027,7 @@
         <f aca="false">SUM(S22:W22)</f>
         <v>2.5</v>
       </c>
-      <c r="P22" s="21" t="inlineStr">
+      <c r="P22" s="20" t="inlineStr">
         <f aca="false">F22</f>
         <is>
           <t/>
@@ -7092,7 +7091,7 @@
         <f aca="false">SUM(S23:W23)</f>
         <v>6.25</v>
       </c>
-      <c r="P23" s="21" t="inlineStr">
+      <c r="P23" s="20" t="inlineStr">
         <f aca="false">F23</f>
         <is>
           <t/>
@@ -7156,7 +7155,7 @@
         <f aca="false">SUM(S24:W24)</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="P24" s="21" t="inlineStr">
+      <c r="P24" s="20" t="inlineStr">
         <f aca="false">F24</f>
         <is>
           <t/>
@@ -7211,7 +7210,7 @@
         <f aca="false">SUM(S25:W25)</f>
         <v>1.25</v>
       </c>
-      <c r="P25" s="21" t="inlineStr">
+      <c r="P25" s="20" t="inlineStr">
         <f aca="false">F25</f>
         <is>
           <t/>
@@ -7234,7 +7233,7 @@
       <c r="A26" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -7272,7 +7271,7 @@
         <f aca="false">SUM(S26:W26)</f>
         <v>3.66666666666667</v>
       </c>
-      <c r="P26" s="21" t="inlineStr">
+      <c r="P26" s="20" t="inlineStr">
         <f aca="false">F26</f>
         <is>
           <t/>
@@ -7338,22 +7337,22 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="17.0666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.7607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="18.4941176470588"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="25" width="21.4705882352941"/>
-    <col collapsed="false" hidden="true" max="7" min="7" style="25" width="0"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="25" width="21.4705882352941"/>
-    <col collapsed="false" hidden="false" max="1014" min="10" style="23" width="12.7333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="12.8627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="17.2313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="19.9607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.678431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="24" width="21.6901960784314"/>
+    <col collapsed="false" hidden="true" max="7" min="7" style="24" width="0"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="24" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="1014" min="10" style="22" width="12.8627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="12.8627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -7379,39 +7378,39 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="27" t="n">
+      <c r="A2" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="27" t="n">
         <v>41902</v>
       </c>
-      <c r="C2" s="27" t="n">
+      <c r="C2" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D2" s="27" t="n">
+      <c r="D2" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1TDHE)</f>
         <v>36</v>
       </c>
-      <c r="E2" s="29" t="n">
+      <c r="E2" s="28" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1PIDGE)</f>
         <v>0.369230769230769</v>
       </c>
-      <c r="F2" s="29" t="inlineStr">
+      <c r="F2" s="28" t="inlineStr">
         <f aca="false">E2</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G2" s="29" t="n">
+      <c r="G2" s="28" t="n">
         <f aca="false">SUMIF(_1SR,A2,_1TDHT)</f>
         <v>17.65</v>
       </c>
-      <c r="H2" s="29" t="n">
+      <c r="H2" s="28" t="n">
         <f aca="false">SUMIF(_1SR,A2,_1PIDGO)</f>
         <v>0.235897435897436</v>
       </c>
-      <c r="I2" s="29" t="inlineStr">
+      <c r="I2" s="28" t="inlineStr">
         <f aca="false">H2</f>
         <is>
           <t/>
@@ -7419,42 +7418,42 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="27" t="n">
+      <c r="A3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="inlineStr">
+      <c r="B3" s="27" t="inlineStr">
         <f aca="false">B2+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1TDHE)</f>
         <v>33.5</v>
       </c>
-      <c r="E3" s="29" t="n">
+      <c r="E3" s="28" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1PIDGE)</f>
         <v>0.343589743589744</v>
       </c>
-      <c r="F3" s="29" t="inlineStr">
+      <c r="F3" s="28" t="inlineStr">
         <f aca="false">E3+F2</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G3" s="29" t="n">
+      <c r="G3" s="28" t="n">
         <f aca="false">SUMIF(_1SR,A3,_1TDHT)</f>
         <v>15.1166666666667</v>
       </c>
-      <c r="H3" s="29" t="n">
+      <c r="H3" s="28" t="n">
         <f aca="false">SUMIF(_1SR,A3,_1PIDGO)</f>
         <v>0.138461538461539</v>
       </c>
-      <c r="I3" s="29" t="inlineStr">
+      <c r="I3" s="28" t="inlineStr">
         <f aca="false">H3+I2</f>
         <is>
           <t/>
@@ -7462,42 +7461,42 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="27" t="n">
+      <c r="A4" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="inlineStr">
+      <c r="B4" s="27" t="inlineStr">
         <f aca="false">B3+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="26" t="n">
         <f aca="false">7*5</f>
         <v>35</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1TDHE)</f>
         <v>28</v>
       </c>
-      <c r="E4" s="29" t="n">
+      <c r="E4" s="28" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1PIDGE)</f>
         <v>0.287179487179487</v>
       </c>
-      <c r="F4" s="29" t="inlineStr">
+      <c r="F4" s="28" t="inlineStr">
         <f aca="false">E4+F3</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G4" s="29" t="n">
+      <c r="G4" s="28" t="n">
         <f aca="false">SUMIF(_1SR,A4,_1TDHT)</f>
         <v>39.8833333333333</v>
       </c>
-      <c r="H4" s="29" t="n">
+      <c r="H4" s="28" t="n">
         <f aca="false">SUMIF(_1SR,A4,_1PIDGO)</f>
         <v>0.36923076923077</v>
       </c>
-      <c r="I4" s="29" t="inlineStr">
+      <c r="I4" s="28" t="inlineStr">
         <f aca="false">H4+I3</f>
         <is>
           <t/>
@@ -7505,18 +7504,18 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="22" t="n">
         <f aca="false">SUM(C2:C4)</f>
         <v>105</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="22" t="n">
         <f aca="false">SUM(D2:D4)</f>
         <v>97.5</v>
       </c>
-      <c r="G6" s="25" t="inlineStr">
+      <c r="G6" s="24" t="inlineStr">
         <f aca="false">SUM(G2:G4)</f>
         <is>
           <t/>
@@ -7542,16 +7541,16 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="G38" activeCellId="0" pane="topLeft" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="23" width="15.7098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="2.6156862745098"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="23" width="15.7098039215686"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="23" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="22" width="15.8745098039216"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="2.65098039215686"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="22" width="15.8745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="22" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1">
@@ -7596,199 +7595,199 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="27" t="n">
+      <c r="A2" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hetl)</f>
         <v>6.5</v>
       </c>
-      <c r="C2" s="27" t="n">
+      <c r="C2" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hedm)</f>
         <v>7</v>
       </c>
-      <c r="D2" s="27" t="n">
+      <c r="D2" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hepqm)</f>
         <v>5.5</v>
       </c>
-      <c r="E2" s="27" t="n">
+      <c r="E2" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hepm)</f>
         <v>11.5</v>
       </c>
-      <c r="F2" s="27" t="n">
+      <c r="F2" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A2,_1hesm)</f>
         <v>5.5</v>
       </c>
-      <c r="G2" s="27" t="n">
+      <c r="G2" s="26" t="n">
         <f aca="false">SUM(B2:F2)</f>
         <v>36</v>
       </c>
-      <c r="I2" s="27" t="n">
+      <c r="I2" s="26" t="n">
         <v>2.35</v>
       </c>
-      <c r="J2" s="27" t="n">
+      <c r="J2" s="26" t="n">
         <v>2.1</v>
       </c>
-      <c r="K2" s="27" t="n">
+      <c r="K2" s="26" t="n">
         <v>3.93</v>
       </c>
-      <c r="L2" s="27" t="n">
+      <c r="L2" s="26" t="n">
         <v>7.42</v>
       </c>
-      <c r="M2" s="27" t="n">
+      <c r="M2" s="26" t="n">
         <v>5.27</v>
       </c>
-      <c r="N2" s="27" t="n">
+      <c r="N2" s="26" t="n">
         <f aca="false">SUM(I2:M2)</f>
         <v>21.07</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="27" t="n">
+      <c r="A3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="n">
+      <c r="B3" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hetl)</f>
         <v>5</v>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hedm)</f>
         <v>10</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hepqm)</f>
         <v>7</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hepm)</f>
         <v>6.5</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A3,_1hesm)</f>
         <v>5</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <f aca="false">SUM(B3:F3)</f>
         <v>33.5</v>
       </c>
-      <c r="I3" s="27" t="n">
+      <c r="I3" s="26" t="n">
         <v>7.33</v>
       </c>
-      <c r="J3" s="27" t="n">
+      <c r="J3" s="26" t="n">
         <v>7.28</v>
       </c>
-      <c r="K3" s="27" t="n">
+      <c r="K3" s="26" t="n">
         <v>5.33</v>
       </c>
-      <c r="L3" s="27" t="n">
+      <c r="L3" s="26" t="n">
         <v>4.42</v>
       </c>
-      <c r="M3" s="27" t="n">
+      <c r="M3" s="26" t="n">
         <v>4.67</v>
       </c>
-      <c r="N3" s="27" t="n">
+      <c r="N3" s="26" t="n">
         <f aca="false">SUM(I3:M3)</f>
         <v>29.03</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="27" t="n">
+      <c r="A4" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="n">
+      <c r="B4" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hetl)</f>
         <v>8.5</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hedm)</f>
         <v>9.5</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hepqm)</f>
         <v>3</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hepm)</f>
         <v>3</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <f aca="false">SUMIF(_1SE,A4,_1hesm)</f>
         <v>4</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <f aca="false">SUM(B4:F4)</f>
         <v>28</v>
       </c>
-      <c r="I4" s="27" t="n">
+      <c r="I4" s="26" t="n">
         <v>5.43</v>
       </c>
-      <c r="J4" s="27" t="n">
+      <c r="J4" s="26" t="n">
         <v>8.72</v>
       </c>
-      <c r="K4" s="27" t="n">
+      <c r="K4" s="26" t="n">
         <v>10.12</v>
       </c>
-      <c r="L4" s="27" t="n">
+      <c r="L4" s="26" t="n">
         <v>10.5</v>
       </c>
-      <c r="M4" s="27" t="n">
+      <c r="M4" s="26" t="n">
         <v>5.87</v>
       </c>
-      <c r="N4" s="27" t="n">
+      <c r="N4" s="26" t="n">
         <f aca="false">SUM(I4:M4)</f>
         <v>40.64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5" s="23"/>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5" s="22"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="22" t="n">
         <f aca="false">SUM(B2:B4)</f>
         <v>20</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="22" t="n">
         <f aca="false">SUM(C2:C4)</f>
         <v>26.5</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="22" t="n">
         <f aca="false">SUM(D2:D4)</f>
         <v>15.5</v>
       </c>
-      <c r="E6" s="23" t="n">
+      <c r="E6" s="22" t="n">
         <f aca="false">SUM(E2:E4)</f>
         <v>21</v>
       </c>
-      <c r="F6" s="23" t="n">
+      <c r="F6" s="22" t="n">
         <f aca="false">SUM(F2:F4)</f>
         <v>14.5</v>
       </c>
-      <c r="G6" s="23" t="n">
+      <c r="G6" s="22" t="n">
         <f aca="false">SUM(G2:G4)</f>
         <v>97.5</v>
       </c>
-      <c r="I6" s="23" t="n">
+      <c r="I6" s="22" t="n">
         <f aca="false">SUM(I2:I4)</f>
         <v>15.11</v>
       </c>
-      <c r="J6" s="23" t="n">
+      <c r="J6" s="22" t="n">
         <f aca="false">SUM(J2:J4)</f>
         <v>18.1</v>
       </c>
-      <c r="K6" s="23" t="n">
+      <c r="K6" s="22" t="n">
         <f aca="false">SUM(K2:K4)</f>
         <v>19.38</v>
       </c>
-      <c r="L6" s="23" t="n">
+      <c r="L6" s="22" t="n">
         <f aca="false">SUM(L2:L4)</f>
         <v>22.34</v>
       </c>
-      <c r="M6" s="23" t="n">
+      <c r="M6" s="22" t="n">
         <f aca="false">SUM(M2:M4)</f>
         <v>15.81</v>
       </c>
-      <c r="N6" s="23" t="n">
+      <c r="N6" s="22" t="n">
         <f aca="false">SUM(N2:N4)</f>
         <v>90.74</v>
       </c>

</xml_diff>

<commit_message>
Actualización del sistema de archivos del proyecto
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -13,13 +13,15 @@
     <sheet name="1" sheetId="3" r:id="rId4"/>
     <sheet name="2" sheetId="4" r:id="rId5"/>
     <sheet name="3" sheetId="6" r:id="rId6"/>
+    <sheet name="1-ganancias" sheetId="7" r:id="rId7"/>
+    <sheet name="2-ganancias" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="146">
   <si>
     <t>Semana</t>
   </si>
@@ -884,24 +886,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="72039424"/>
-        <c:axId val="72045312"/>
+        <c:axId val="77680000"/>
+        <c:axId val="77685888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72039424"/>
+        <c:axId val="77680000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72045312"/>
+        <c:crossAx val="77685888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72045312"/>
+        <c:axId val="77685888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +911,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72039424"/>
+        <c:crossAx val="77680000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -922,7 +924,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1051,24 +1053,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="135852800"/>
-        <c:axId val="137906816"/>
+        <c:axId val="77706368"/>
+        <c:axId val="77707904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135852800"/>
+        <c:axId val="77706368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137906816"/>
+        <c:crossAx val="77707904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137906816"/>
+        <c:axId val="77707904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,7 +1078,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135852800"/>
+        <c:crossAx val="77706368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1089,7 +1091,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1275,24 +1277,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72357760"/>
-        <c:axId val="72359296"/>
+        <c:axId val="77873152"/>
+        <c:axId val="77874688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72357760"/>
+        <c:axId val="77873152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72359296"/>
+        <c:crossAx val="77874688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72359296"/>
+        <c:axId val="77874688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1302,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72357760"/>
+        <c:crossAx val="77873152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1313,7 +1315,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1385,24 +1387,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="102144256"/>
-        <c:axId val="102158336"/>
+        <c:axId val="77908224"/>
+        <c:axId val="77914112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102144256"/>
+        <c:axId val="77908224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102158336"/>
+        <c:crossAx val="77914112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102158336"/>
+        <c:axId val="77914112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,7 +1412,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102144256"/>
+        <c:crossAx val="77908224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1423,7 +1425,471 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1-ganancias'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje acumulado de ganancias estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1-ganancias'!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.36923076923076925</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71282051282051273</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1-ganancias'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje acumulado de ganancias obtenidas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1-ganancias'!$H$2:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.23589743589743592</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37435897435897436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74358974358974361</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="65288448"/>
+        <c:axId val="65298432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="65288448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65298432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65298432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1-ganancias'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje individual de ganancias estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1-ganancias'!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.36923076923076925</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34358974358974353</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28717948717948716</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1-ganancias'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje individual de ganancias obtenidas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1-ganancias'!$G$2:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.23589743589743592</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3692307692307692</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="67223552"/>
+        <c:axId val="67225088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="67223552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67225088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="67225088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67223552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2-ganancias'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje acumulado de ganancias estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'2-ganancias'!$E$2:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.51094890510948909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2-ganancias'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje acumulado de ganancias obtenidas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'2-ganancias'!$H$2:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.36496350364963503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96350364963503654</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="64504576"/>
+        <c:axId val="64506112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="64504576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64506112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="64506112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64504576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2-ganancias'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje individual de ganancias estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'2-ganancias'!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.51094890510948909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48905109489051102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2-ganancias'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje individual de ganancias obtenidas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'2-ganancias'!$G$2:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.36496350364963503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59854014598540151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="64530688"/>
+        <c:axId val="64532480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="64530688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64532480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="64532480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64530688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1499,13 +1965,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:colOff>200023</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
@@ -1529,19 +1995,149 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>200026</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1846,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2194,8 +2790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2861,8 +3457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="12.75"/>
@@ -52233,7 +52829,7 @@
   <dimension ref="A1:AMK28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -52785,7 +53381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" ht="25.5">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -53244,7 +53840,7 @@
         <v>1.1944444444444442</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="25.5">
+    <row r="16" spans="1:24" ht="38.25">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -53368,7 +53964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" ht="25.5">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -53508,7 +54104,7 @@
         <v>1.6333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="25.5">
+    <row r="20" spans="1:24" ht="38.25">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -53567,7 +54163,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" ht="25.5">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -53630,7 +54226,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="25.5">
+    <row r="22" spans="1:24" ht="38.25">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -53693,7 +54289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="25.5">
+    <row r="23" spans="1:24" ht="51">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -53756,7 +54352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="25.5">
+    <row r="24" spans="1:24" ht="63.75">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -53851,8 +54447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -53936,7 +54532,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" ht="38.25">
       <c r="A2" s="18">
         <v>24</v>
       </c>
@@ -54208,7 +54804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="38.25">
+    <row r="6" spans="1:24" ht="51">
       <c r="A6" s="18">
         <v>28</v>
       </c>
@@ -55637,4 +56233,246 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="32" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="32" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="57">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3">
+        <f>ganancias!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <f>LOOKUP(A2,ganancias!A:A,ganancias!B:B)</f>
+        <v>41902</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="5">
+        <f>SUMIF('1'!$G:$G,A2,'1'!$F:$F)</f>
+        <v>0.36923076923076925</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2</f>
+        <v>0.36923076923076925</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="6">
+        <f>SUMIF('1'!$R:$R,A2,'1'!$Q:$Q)</f>
+        <v>0.23589743589743592</v>
+      </c>
+      <c r="H2" s="6">
+        <f>G2</f>
+        <v>0.23589743589743592</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3">
+        <f>ganancias!A3</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <f>LOOKUP(A3,ganancias!A:A,ganancias!B:B)</f>
+        <v>41909</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="5">
+        <f>SUMIF('1'!$G:$G,A3,'1'!$F:$F)</f>
+        <v>0.34358974358974353</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E4" si="0">D3+E2</f>
+        <v>0.71282051282051273</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="6">
+        <f>SUMIF('1'!$R:$R,A3,'1'!$Q:$Q)</f>
+        <v>0.13846153846153847</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" ref="H3:H4" si="1">G3+H2</f>
+        <v>0.37435897435897436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3">
+        <f>ganancias!A4</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <f>LOOKUP(A4,ganancias!A:A,ganancias!B:B)</f>
+        <v>41916</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="5">
+        <f>SUMIF('1'!$G:$G,A4,'1'!$F:$F)</f>
+        <v>0.28717948717948716</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="6">
+        <f>SUMIF('1'!$R:$R,A4,'1'!$Q:$Q)</f>
+        <v>0.3692307692307692</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.74358974358974361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="32" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="32" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="57">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3">
+        <f>ganancias!A5</f>
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <f>LOOKUP(A2,ganancias!A:A,ganancias!B:B)</f>
+        <v>41923</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="5">
+        <f>SUMIF('2'!$G:$G,A2,'2'!$F:$F)</f>
+        <v>0.51094890510948909</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2</f>
+        <v>0.51094890510948909</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="6">
+        <f>SUMIF('2'!$R:$R,A2,'2'!$Q:$Q)</f>
+        <v>0.36496350364963503</v>
+      </c>
+      <c r="H2" s="6">
+        <f>G2</f>
+        <v>0.36496350364963503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3">
+        <f>ganancias!A6</f>
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <f>LOOKUP(A3,ganancias!A:A,ganancias!B:B)</f>
+        <v>41930</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="5">
+        <f>SUMIF('2'!$G:$G,A3,'2'!$F:$F)</f>
+        <v>0.48905109489051102</v>
+      </c>
+      <c r="E3" s="6">
+        <f>D3+E2</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="6">
+        <f>SUMIF('2'!$R:$R,A3,'2'!$Q:$Q)</f>
+        <v>0.59854014598540151</v>
+      </c>
+      <c r="H3" s="6">
+        <f>G3+H2</f>
+        <v>0.96350364963503654</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización del mockup de adr
Asignación disponibilidad recursos
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\pucmm\isc-434-t\ppr\tspi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\github\PPR\tspi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="-15" windowWidth="9540" windowHeight="3690" tabRatio="516" activeTab="1"/>
+    <workbookView xWindow="9705" yWindow="-15" windowWidth="9540" windowHeight="3690" tabRatio="516" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ganancias" sheetId="1" r:id="rId1"/>
@@ -1018,11 +1018,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1118757152"/>
-        <c:axId val="-1118756064"/>
+        <c:axId val="1990185696"/>
+        <c:axId val="1990193856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1118757152"/>
+        <c:axId val="1990185696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,7 +1031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1118756064"/>
+        <c:crossAx val="1990193856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1039,7 +1039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1118756064"/>
+        <c:axId val="1990193856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1118757152"/>
+        <c:crossAx val="1990185696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1218,11 +1218,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1118753344"/>
-        <c:axId val="-1118751712"/>
+        <c:axId val="2105737008"/>
+        <c:axId val="2105749520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1118753344"/>
+        <c:axId val="2105737008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1118751712"/>
+        <c:crossAx val="2105749520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1118751712"/>
+        <c:axId val="2105749520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1118753344"/>
+        <c:crossAx val="2105737008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1418,8 +1418,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-981170400"/>
-        <c:axId val="-981172576"/>
+        <c:axId val="2105751152"/>
+        <c:axId val="2105744080"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1495,11 +1495,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-981170400"/>
-        <c:axId val="-981172576"/>
+        <c:axId val="2105751152"/>
+        <c:axId val="2105744080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-981170400"/>
+        <c:axId val="2105751152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,7 +1508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981172576"/>
+        <c:crossAx val="2105744080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1516,7 +1516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-981172576"/>
+        <c:axId val="2105744080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,7 +1527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981170400"/>
+        <c:crossAx val="2105751152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1639,11 +1639,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-981174752"/>
-        <c:axId val="-981179648"/>
+        <c:axId val="2105738096"/>
+        <c:axId val="2105748976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-981174752"/>
+        <c:axId val="2105738096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1652,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981179648"/>
+        <c:crossAx val="2105748976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1660,7 +1660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-981179648"/>
+        <c:axId val="2105748976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,14 +1671,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981174752"/>
+        <c:crossAx val="2105738096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1791,11 +1790,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-981176928"/>
-        <c:axId val="-981176384"/>
+        <c:axId val="2105742992"/>
+        <c:axId val="2105738640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-981176928"/>
+        <c:axId val="2105742992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,7 +1803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981176384"/>
+        <c:crossAx val="2105738640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1812,7 +1811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-981176384"/>
+        <c:axId val="2105738640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,14 +1822,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981176928"/>
+        <c:crossAx val="2105742992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1943,11 +1941,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-981177472"/>
-        <c:axId val="-981169312"/>
+        <c:axId val="2105745712"/>
+        <c:axId val="2105744624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-981177472"/>
+        <c:axId val="2105745712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,7 +1954,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981169312"/>
+        <c:crossAx val="2105744624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1964,7 +1962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-981169312"/>
+        <c:axId val="2105744624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,14 +1973,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981177472"/>
+        <c:crossAx val="2105745712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2089,11 +2086,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-981174208"/>
-        <c:axId val="-981181280"/>
+        <c:axId val="2105746256"/>
+        <c:axId val="2105747888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-981174208"/>
+        <c:axId val="2105746256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2102,7 +2099,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981181280"/>
+        <c:crossAx val="2105747888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2110,7 +2107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-981181280"/>
+        <c:axId val="2105747888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2121,14 +2118,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981174208"/>
+        <c:crossAx val="2105746256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2235,11 +2231,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-981167680"/>
-        <c:axId val="-981178560"/>
+        <c:axId val="2105740816"/>
+        <c:axId val="2105748432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-981167680"/>
+        <c:axId val="2105740816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2248,7 +2244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981178560"/>
+        <c:crossAx val="2105748432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2256,7 +2252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-981178560"/>
+        <c:axId val="2105748432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2267,14 +2263,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-981167680"/>
+        <c:crossAx val="2105740816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2838,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3186,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3853,8 +3848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK69"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Versión final del sds, actualización srs Falta escribir al conclusión del sds
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -1018,11 +1018,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1990185696"/>
-        <c:axId val="1990193856"/>
+        <c:axId val="-770839504"/>
+        <c:axId val="-770836784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1990185696"/>
+        <c:axId val="-770839504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,7 +1031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1990193856"/>
+        <c:crossAx val="-770836784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1039,7 +1039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1990193856"/>
+        <c:axId val="-770836784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1990185696"/>
+        <c:crossAx val="-770839504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1218,11 +1218,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105737008"/>
-        <c:axId val="2105749520"/>
+        <c:axId val="-770840048"/>
+        <c:axId val="-770830256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105737008"/>
+        <c:axId val="-770840048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105749520"/>
+        <c:crossAx val="-770830256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105749520"/>
+        <c:axId val="-770830256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105737008"/>
+        <c:crossAx val="-770840048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1418,8 +1418,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105751152"/>
-        <c:axId val="2105744080"/>
+        <c:axId val="-770835152"/>
+        <c:axId val="-770833520"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1495,11 +1495,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105751152"/>
-        <c:axId val="2105744080"/>
+        <c:axId val="-770835152"/>
+        <c:axId val="-770833520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105751152"/>
+        <c:axId val="-770835152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,7 +1508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105744080"/>
+        <c:crossAx val="-770833520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1516,7 +1516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105744080"/>
+        <c:axId val="-770833520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,7 +1527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105751152"/>
+        <c:crossAx val="-770835152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1639,11 +1639,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105738096"/>
-        <c:axId val="2105748976"/>
+        <c:axId val="-770831888"/>
+        <c:axId val="-770826992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105738096"/>
+        <c:axId val="-770831888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1652,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105748976"/>
+        <c:crossAx val="-770826992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1660,7 +1660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105748976"/>
+        <c:axId val="-770826992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,13 +1671,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105738096"/>
+        <c:crossAx val="-770831888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1790,11 +1791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105742992"/>
-        <c:axId val="2105738640"/>
+        <c:axId val="-770829712"/>
+        <c:axId val="-770828080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105742992"/>
+        <c:axId val="-770829712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,7 +1804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105738640"/>
+        <c:crossAx val="-770828080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1811,7 +1812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105738640"/>
+        <c:axId val="-770828080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1822,7 +1823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105742992"/>
+        <c:crossAx val="-770829712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1941,11 +1942,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105745712"/>
-        <c:axId val="2105744624"/>
+        <c:axId val="-655027920"/>
+        <c:axId val="-655020304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105745712"/>
+        <c:axId val="-655027920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +1955,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105744624"/>
+        <c:crossAx val="-655020304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1962,7 +1963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105744624"/>
+        <c:axId val="-655020304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105745712"/>
+        <c:crossAx val="-655027920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2086,11 +2087,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105746256"/>
-        <c:axId val="2105747888"/>
+        <c:axId val="-655030640"/>
+        <c:axId val="-655035536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105746256"/>
+        <c:axId val="-655030640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105747888"/>
+        <c:crossAx val="-655035536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2107,7 +2108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105747888"/>
+        <c:axId val="-655035536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2118,7 +2119,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105746256"/>
+        <c:crossAx val="-655030640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2231,11 +2232,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105740816"/>
-        <c:axId val="2105748432"/>
+        <c:axId val="-655023024"/>
+        <c:axId val="-655034992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105740816"/>
+        <c:axId val="-655023024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,7 +2245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105748432"/>
+        <c:crossAx val="-655034992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2252,7 +2253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105748432"/>
+        <c:axId val="-655034992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2263,7 +2264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105740816"/>
+        <c:crossAx val="-655023024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2833,7 +2834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3181,7 +3182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -3848,8 +3849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
PM Report y peer review
</commit_message>
<xml_diff>
--- a/tspi/plan.xlsx
+++ b/tspi/plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="-15" windowWidth="9540" windowHeight="3690" tabRatio="585"/>
+    <workbookView xWindow="9705" yWindow="-15" windowWidth="9540" windowHeight="3690" tabRatio="585" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ganancias" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="182">
   <si>
     <t>Semana</t>
   </si>
@@ -571,6 +571,9 @@
   <si>
     <t>Elaborar el plan del ciclo #4.</t>
   </si>
+  <si>
+    <t>Desarrollar la funcionalidad que permite establecer la disponibilidad en horas por día a los recursos.</t>
+  </si>
 </sst>
 </file>
 
@@ -1028,11 +1031,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108961296"/>
-        <c:axId val="108948784"/>
+        <c:axId val="983940736"/>
+        <c:axId val="983934752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108961296"/>
+        <c:axId val="983940736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108948784"/>
+        <c:crossAx val="983934752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108948784"/>
+        <c:axId val="983934752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108961296"/>
+        <c:crossAx val="983940736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,11 +1207,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108931296"/>
-        <c:axId val="108939456"/>
+        <c:axId val="1106562096"/>
+        <c:axId val="1106564816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108931296"/>
+        <c:axId val="1106562096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108939456"/>
+        <c:crossAx val="1106564816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1226,7 +1229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108939456"/>
+        <c:axId val="1106564816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108931296"/>
+        <c:crossAx val="1106562096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1405,11 +1408,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108958032"/>
-        <c:axId val="108951504"/>
+        <c:axId val="983931488"/>
+        <c:axId val="983932032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108958032"/>
+        <c:axId val="983931488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1418,7 +1421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108951504"/>
+        <c:crossAx val="983932032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1426,7 +1429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108951504"/>
+        <c:axId val="983932032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108958032"/>
+        <c:crossAx val="983931488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1605,8 +1608,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108950416"/>
-        <c:axId val="108954224"/>
+        <c:axId val="983935840"/>
+        <c:axId val="983936384"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1682,11 +1685,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108950416"/>
-        <c:axId val="108954224"/>
+        <c:axId val="983935840"/>
+        <c:axId val="983936384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108950416"/>
+        <c:axId val="983935840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1695,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108954224"/>
+        <c:crossAx val="983936384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1703,7 +1706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108954224"/>
+        <c:axId val="983936384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108950416"/>
+        <c:crossAx val="983935840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1826,11 +1829,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108959664"/>
-        <c:axId val="108956400"/>
+        <c:axId val="983926592"/>
+        <c:axId val="983938016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108959664"/>
+        <c:axId val="983926592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1839,7 +1842,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108956400"/>
+        <c:crossAx val="983938016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1847,7 +1850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108956400"/>
+        <c:axId val="983938016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,7 +1861,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108959664"/>
+        <c:crossAx val="983926592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1978,11 +1981,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108953136"/>
-        <c:axId val="108948240"/>
+        <c:axId val="983938560"/>
+        <c:axId val="983940192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108953136"/>
+        <c:axId val="983938560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,7 +1994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108948240"/>
+        <c:crossAx val="983940192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1999,7 +2002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108948240"/>
+        <c:axId val="983940192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2010,7 +2013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108953136"/>
+        <c:crossAx val="983938560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2130,11 +2133,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108955312"/>
-        <c:axId val="108956944"/>
+        <c:axId val="983928768"/>
+        <c:axId val="1106561552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108955312"/>
+        <c:axId val="983928768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108956944"/>
+        <c:crossAx val="1106561552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2151,7 +2154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108956944"/>
+        <c:axId val="1106561552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,7 +2165,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108955312"/>
+        <c:crossAx val="983928768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2276,11 +2279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108935104"/>
-        <c:axId val="108934016"/>
+        <c:axId val="1106558832"/>
+        <c:axId val="1106566448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108935104"/>
+        <c:axId val="1106558832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2289,7 +2292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108934016"/>
+        <c:crossAx val="1106566448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2297,7 +2300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108934016"/>
+        <c:axId val="1106566448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2308,7 +2311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108935104"/>
+        <c:crossAx val="1106558832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2422,11 +2425,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108940000"/>
-        <c:axId val="108944896"/>
+        <c:axId val="1106571344"/>
+        <c:axId val="1106567536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108940000"/>
+        <c:axId val="1106571344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,7 +2438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108944896"/>
+        <c:crossAx val="1106567536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2443,7 +2446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108944896"/>
+        <c:axId val="1106567536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2454,7 +2457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108940000"/>
+        <c:crossAx val="1106571344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2644,11 +2647,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108931840"/>
-        <c:axId val="108932928"/>
+        <c:axId val="1106569168"/>
+        <c:axId val="1106563184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108931840"/>
+        <c:axId val="1106569168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2658,7 +2661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108932928"/>
+        <c:crossAx val="1106563184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2666,7 +2669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108932928"/>
+        <c:axId val="1106563184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,7 +2680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108931840"/>
+        <c:crossAx val="1106569168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3317,8 +3320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3665,8 +3668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4360,10 +4363,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK73"/>
+  <dimension ref="A1:AMK75"/>
   <sheetViews>
-    <sheetView topLeftCell="C64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -55307,6 +55310,19 @@
         <v>8</v>
       </c>
     </row>
+    <row r="74" spans="1:1025" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="16">
+        <v>70</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1025" x14ac:dyDescent="0.2">
+      <c r="A75" s="16">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -60159,8 +60175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>